<commit_message>
Added large quantity pricing for relevant components, still missing some parts
</commit_message>
<xml_diff>
--- a/PCB-Node1/BOM_BYGGERNNODE1.xlsx
+++ b/PCB-Node1/BOM_BYGGERNNODE1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benja\Documents\Byggeren\TTK4155_Ping_Pong_Project\PCB-Node1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01EAF227-BCEF-4021-9A06-4F125C210720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2211120-BBFF-433A-80C4-2932D5698227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{17AFD791-CEED-4828-96C0-A0F19B8C3E72}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="136">
   <si>
     <t>Byggern 2024 Node 1   Revised: Monday, October 21, 2024</t>
   </si>
@@ -432,6 +432,15 @@
   </si>
   <si>
     <t>https://www.digikey.no/en/products/detail/w%C3%BCrth-elektronik/691418320002/11477851?s=N4IgTCBcDaIGwE4CMAWJAOAzGADHiAugL5A</t>
+  </si>
+  <si>
+    <t>10pc cost</t>
+  </si>
+  <si>
+    <t>50pc cost</t>
+  </si>
+  <si>
+    <t>Order cost</t>
   </si>
 </sst>
 </file>
@@ -1316,10 +1325,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D679CB1F-3136-4EF7-BB0E-65C07665A41B}">
-  <dimension ref="A1:L55"/>
+  <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1327,24 +1336,26 @@
     <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.1796875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.6328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.36328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="90" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.90625" customWidth="1"/>
+    <col min="10" max="10" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.6328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="90" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1352,7 +1363,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1375,27 +1386,36 @@
         <v>10</v>
       </c>
       <c r="H12" t="s">
+        <v>133</v>
+      </c>
+      <c r="I12" t="s">
+        <v>134</v>
+      </c>
+      <c r="J12" t="s">
         <v>11</v>
       </c>
-      <c r="I12" t="s">
+      <c r="K12" t="s">
         <v>12</v>
       </c>
-      <c r="J12" t="s">
+      <c r="L12" t="s">
         <v>13</v>
       </c>
-      <c r="K12" t="s">
+      <c r="M12" t="s">
+        <v>135</v>
+      </c>
+      <c r="N12" t="s">
         <v>14</v>
       </c>
-      <c r="L12" t="s">
+      <c r="O12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1417,23 +1437,29 @@
       <c r="G15" s="2">
         <v>12.81</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2">
         <v>25.62</v>
       </c>
-      <c r="I15" s="2">
+      <c r="K15" s="2">
         <v>76.86</v>
       </c>
-      <c r="J15" s="2">
+      <c r="L15" s="2">
         <v>76.86</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="M15" s="2">
+        <f>IF(D15&gt;=50,D15*I15,IF(D15&gt;=10,D15*H15,D15*G15))</f>
+        <v>76.86</v>
+      </c>
+      <c r="N15" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="L15" t="s">
+      <c r="O15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1455,23 +1481,29 @@
       <c r="G16" s="2">
         <v>10.19</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2">
         <v>10.19</v>
       </c>
-      <c r="I16" s="2">
+      <c r="K16" s="2">
         <v>30.57</v>
       </c>
-      <c r="J16" s="2">
+      <c r="L16" s="2">
         <v>50.95</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="M16" s="2">
+        <f t="shared" ref="M16:M48" si="0">IF(D16&gt;=50,D16*I16,IF(D16&gt;=10,D16*H16,D16*G16))</f>
+        <v>50.949999999999996</v>
+      </c>
+      <c r="N16" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="L16" t="s">
+      <c r="O16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>3</v>
       </c>
@@ -1493,23 +1525,29 @@
       <c r="G17" s="2">
         <v>5.99</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2">
         <v>5.99</v>
       </c>
-      <c r="I17" s="2">
+      <c r="K17" s="2">
         <v>17.97</v>
       </c>
-      <c r="J17" s="2">
+      <c r="L17" s="2">
         <v>29.95</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="M17" s="2">
+        <f t="shared" si="0"/>
+        <v>29.950000000000003</v>
+      </c>
+      <c r="N17" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="L17" t="s">
+      <c r="O17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>4</v>
       </c>
@@ -1532,22 +1570,32 @@
         <v>2</v>
       </c>
       <c r="H18" s="2">
+        <v>1.859</v>
+      </c>
+      <c r="I18" s="2">
+        <v>1.859</v>
+      </c>
+      <c r="J18" s="2">
         <v>30</v>
       </c>
-      <c r="I18" s="2">
+      <c r="K18" s="2">
         <v>90</v>
       </c>
-      <c r="J18" s="2">
+      <c r="L18" s="2">
         <v>100</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="M18" s="2">
+        <f t="shared" si="0"/>
+        <v>92.95</v>
+      </c>
+      <c r="N18" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="L18" t="s">
+      <c r="O18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="C19">
         <v>0</v>
       </c>
@@ -1555,17 +1603,23 @@
         <v>27</v>
       </c>
       <c r="G19" s="2"/>
-      <c r="H19" s="2">
-        <v>0</v>
-      </c>
-      <c r="I19" s="2">
-        <v>0</v>
-      </c>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
       <c r="J19" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K19" s="2">
+        <v>0</v>
+      </c>
+      <c r="L19" s="2">
+        <v>0</v>
+      </c>
+      <c r="M19" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="C20">
         <v>0</v>
       </c>
@@ -1573,17 +1627,23 @@
         <v>28</v>
       </c>
       <c r="G20" s="2"/>
-      <c r="H20" s="2">
-        <v>0</v>
-      </c>
-      <c r="I20" s="2">
-        <v>0</v>
-      </c>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
       <c r="J20" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K20" s="2">
+        <v>0</v>
+      </c>
+      <c r="L20" s="2">
+        <v>0</v>
+      </c>
+      <c r="M20" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>5</v>
       </c>
@@ -1606,22 +1666,32 @@
         <v>1.26</v>
       </c>
       <c r="H21" s="2">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="I21" s="2">
+        <v>0.50619999999999998</v>
+      </c>
+      <c r="J21" s="2">
         <v>13.86</v>
       </c>
-      <c r="I21" s="2">
+      <c r="K21" s="2">
         <v>41.58</v>
       </c>
-      <c r="J21" s="2">
+      <c r="L21" s="2">
         <v>63</v>
       </c>
-      <c r="K21" t="s">
+      <c r="M21" s="2">
+        <f t="shared" si="0"/>
+        <v>25.31</v>
+      </c>
+      <c r="N21" t="s">
         <v>31</v>
       </c>
-      <c r="L21" t="s">
+      <c r="O21" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="C22">
         <v>0</v>
       </c>
@@ -1629,17 +1699,23 @@
         <v>33</v>
       </c>
       <c r="G22" s="2"/>
-      <c r="H22" s="2">
-        <v>0</v>
-      </c>
-      <c r="I22" s="2">
-        <v>0</v>
-      </c>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
       <c r="J22" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K22" s="2">
+        <v>0</v>
+      </c>
+      <c r="L22" s="2">
+        <v>0</v>
+      </c>
+      <c r="M22" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>6</v>
       </c>
@@ -1662,22 +1738,32 @@
         <v>1.05</v>
       </c>
       <c r="H23" s="2">
+        <v>0.83</v>
+      </c>
+      <c r="I23" s="2">
+        <v>0.83</v>
+      </c>
+      <c r="J23" s="2">
         <v>2.1</v>
       </c>
-      <c r="I23" s="2">
+      <c r="K23" s="2">
         <v>6.3</v>
       </c>
-      <c r="J23" s="2">
+      <c r="L23" s="2">
         <v>10.5</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="M23" s="2">
+        <f t="shared" si="0"/>
+        <v>8.2999999999999989</v>
+      </c>
+      <c r="N23" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="L23" t="s">
+      <c r="O23" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>7</v>
       </c>
@@ -1699,23 +1785,29 @@
       <c r="G24" s="2">
         <v>11.55</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2">
         <v>11.55</v>
       </c>
-      <c r="I24" s="2">
+      <c r="K24" s="2">
         <v>34.65</v>
       </c>
-      <c r="J24" s="2">
+      <c r="L24" s="2">
         <v>46.2</v>
       </c>
-      <c r="K24" t="s">
+      <c r="M24" s="2">
+        <f t="shared" si="0"/>
+        <v>46.2</v>
+      </c>
+      <c r="N24" t="s">
         <v>39</v>
       </c>
-      <c r="L24" t="s">
+      <c r="O24" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>8</v>
       </c>
@@ -1737,23 +1829,29 @@
       <c r="G25" s="2">
         <v>4.0999999999999996</v>
       </c>
-      <c r="H25" s="2">
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2">
         <v>4.0999999999999996</v>
       </c>
-      <c r="I25" s="2">
+      <c r="K25" s="2">
         <v>12.3</v>
       </c>
-      <c r="J25" s="2">
+      <c r="L25" s="2">
         <v>16.399999999999999</v>
       </c>
-      <c r="K25" t="s">
+      <c r="M25" s="2">
+        <f t="shared" si="0"/>
+        <v>16.399999999999999</v>
+      </c>
+      <c r="N25" t="s">
         <v>43</v>
       </c>
-      <c r="L25" t="s">
+      <c r="O25" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>9</v>
       </c>
@@ -1775,23 +1873,29 @@
       <c r="G26" s="2">
         <v>5.78</v>
       </c>
-      <c r="H26" s="2">
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2">
         <v>5.78</v>
       </c>
-      <c r="I26" s="2">
+      <c r="K26" s="2">
         <v>17.34</v>
       </c>
-      <c r="J26" s="2">
+      <c r="L26" s="2">
         <v>23.12</v>
       </c>
-      <c r="K26" t="s">
+      <c r="M26" s="2">
+        <f t="shared" si="0"/>
+        <v>23.12</v>
+      </c>
+      <c r="N26" t="s">
         <v>47</v>
       </c>
-      <c r="L26" t="s">
+      <c r="O26" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>10</v>
       </c>
@@ -1813,23 +1917,29 @@
       <c r="G27" s="2">
         <v>5.88</v>
       </c>
-      <c r="H27" s="2">
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2">
         <v>5.88</v>
       </c>
-      <c r="I27" s="2">
+      <c r="K27" s="2">
         <v>17.64</v>
       </c>
-      <c r="J27" s="2">
+      <c r="L27" s="2">
         <v>23.52</v>
       </c>
-      <c r="K27" t="s">
+      <c r="M27" s="2">
+        <f t="shared" si="0"/>
+        <v>23.52</v>
+      </c>
+      <c r="N27" t="s">
         <v>51</v>
       </c>
-      <c r="L27" t="s">
+      <c r="O27" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>11</v>
       </c>
@@ -1851,23 +1961,29 @@
       <c r="G28" s="2">
         <v>5.57</v>
       </c>
-      <c r="H28" s="2">
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2">
         <v>5.57</v>
       </c>
-      <c r="I28" s="2">
+      <c r="K28" s="2">
         <v>16.71</v>
       </c>
-      <c r="J28" s="2">
+      <c r="L28" s="2">
         <v>22.28</v>
       </c>
-      <c r="K28" t="s">
+      <c r="M28" s="2">
+        <f t="shared" si="0"/>
+        <v>22.28</v>
+      </c>
+      <c r="N28" t="s">
         <v>55</v>
       </c>
-      <c r="L28" t="s">
+      <c r="O28" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>12</v>
       </c>
@@ -1889,23 +2005,29 @@
       <c r="G29" s="2">
         <v>3.99</v>
       </c>
-      <c r="H29" s="2">
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2">
         <v>3.99</v>
       </c>
-      <c r="I29" s="2">
+      <c r="K29" s="2">
         <v>11.97</v>
       </c>
-      <c r="J29" s="2">
+      <c r="L29" s="2">
         <v>15.96</v>
       </c>
-      <c r="K29" t="s">
+      <c r="M29" s="2">
+        <f t="shared" si="0"/>
+        <v>15.96</v>
+      </c>
+      <c r="N29" t="s">
         <v>59</v>
       </c>
-      <c r="L29" t="s">
+      <c r="O29" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>13</v>
       </c>
@@ -1927,23 +2049,29 @@
       <c r="G30" s="2">
         <v>3.26</v>
       </c>
-      <c r="H30" s="2">
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2">
         <v>3.26</v>
       </c>
-      <c r="I30" s="2">
+      <c r="K30" s="2">
         <v>9.7799999999999994</v>
       </c>
-      <c r="J30" s="2">
+      <c r="L30" s="2">
         <v>13.04</v>
       </c>
-      <c r="K30" t="s">
+      <c r="M30" s="2">
+        <f t="shared" si="0"/>
+        <v>13.04</v>
+      </c>
+      <c r="N30" t="s">
         <v>63</v>
       </c>
-      <c r="L30" t="s">
+      <c r="O30" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>14</v>
       </c>
@@ -1965,23 +2093,29 @@
       <c r="G31" s="2">
         <v>12.39</v>
       </c>
-      <c r="H31" s="2">
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2">
         <v>12.39</v>
       </c>
-      <c r="I31" s="2">
+      <c r="K31" s="2">
         <v>37.17</v>
       </c>
-      <c r="J31" s="2">
+      <c r="L31" s="2">
         <v>49.56</v>
       </c>
-      <c r="K31" t="s">
+      <c r="M31" s="2">
+        <f t="shared" si="0"/>
+        <v>49.56</v>
+      </c>
+      <c r="N31" t="s">
         <v>66</v>
       </c>
-      <c r="L31" t="s">
+      <c r="O31" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>15</v>
       </c>
@@ -2003,23 +2137,29 @@
       <c r="G32" s="2">
         <v>11.55</v>
       </c>
-      <c r="H32" s="2">
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2">
         <v>11.55</v>
       </c>
-      <c r="I32" s="2">
+      <c r="K32" s="2">
         <v>34.65</v>
       </c>
-      <c r="J32" s="2">
+      <c r="L32" s="2">
         <v>46.2</v>
       </c>
-      <c r="K32" s="1" t="s">
+      <c r="M32" s="2">
+        <f t="shared" si="0"/>
+        <v>46.2</v>
+      </c>
+      <c r="N32" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="L32" t="s">
+      <c r="O32" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>16</v>
       </c>
@@ -2041,23 +2181,29 @@
       <c r="G33" s="2">
         <v>17.12</v>
       </c>
-      <c r="H33" s="2">
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2">
         <v>17.12</v>
       </c>
-      <c r="I33" s="2">
+      <c r="K33" s="2">
         <v>51.36</v>
       </c>
-      <c r="J33" s="2">
+      <c r="L33" s="2">
         <v>68.48</v>
       </c>
-      <c r="K33" t="s">
+      <c r="M33" s="2">
+        <f t="shared" si="0"/>
+        <v>68.48</v>
+      </c>
+      <c r="N33" t="s">
         <v>72</v>
       </c>
-      <c r="L33" t="s">
+      <c r="O33" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>17</v>
       </c>
@@ -2079,23 +2225,29 @@
       <c r="G34" s="2">
         <v>4.9400000000000004</v>
       </c>
-      <c r="H34" s="2">
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2">
         <v>4.9400000000000004</v>
       </c>
-      <c r="I34" s="2">
+      <c r="K34" s="2">
         <v>14.82</v>
       </c>
-      <c r="J34" s="2">
+      <c r="L34" s="2">
         <v>19.760000000000002</v>
       </c>
-      <c r="K34" t="s">
+      <c r="M34" s="2">
+        <f t="shared" si="0"/>
+        <v>19.760000000000002</v>
+      </c>
+      <c r="N34" t="s">
         <v>75</v>
       </c>
-      <c r="L34" t="s">
+      <c r="O34" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>18</v>
       </c>
@@ -2118,22 +2270,32 @@
         <v>1.89</v>
       </c>
       <c r="H35" s="2">
+        <v>1.89</v>
+      </c>
+      <c r="I35" s="2">
+        <v>1.8480000000000001</v>
+      </c>
+      <c r="J35" s="2">
         <v>5.67</v>
       </c>
-      <c r="I35" s="2">
+      <c r="K35" s="2">
         <v>17.010000000000002</v>
       </c>
-      <c r="J35" s="2">
+      <c r="L35" s="2">
         <v>28.35</v>
       </c>
-      <c r="K35" t="s">
+      <c r="M35" s="2">
+        <f t="shared" si="0"/>
+        <v>28.349999999999998</v>
+      </c>
+      <c r="N35" t="s">
         <v>78</v>
       </c>
-      <c r="L35" t="s">
+      <c r="O35" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>19</v>
       </c>
@@ -2153,20 +2315,26 @@
         <v>81</v>
       </c>
       <c r="G36" s="2"/>
-      <c r="H36" s="2">
-        <v>0</v>
-      </c>
-      <c r="I36" s="2">
-        <v>0</v>
-      </c>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
       <c r="J36" s="2">
         <v>0</v>
       </c>
-      <c r="K36" t="s">
+      <c r="K36" s="2">
+        <v>0</v>
+      </c>
+      <c r="L36" s="2">
+        <v>0</v>
+      </c>
+      <c r="M36" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N36" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>20</v>
       </c>
@@ -2189,22 +2357,32 @@
         <v>1.05</v>
       </c>
       <c r="H37" s="2">
+        <v>0.41</v>
+      </c>
+      <c r="I37" s="2">
+        <v>0.26040000000000002</v>
+      </c>
+      <c r="J37" s="2">
         <v>5.25</v>
       </c>
-      <c r="I37" s="2">
+      <c r="K37" s="2">
         <v>15.75</v>
       </c>
-      <c r="J37" s="2">
+      <c r="L37" s="2">
         <v>52.5</v>
       </c>
-      <c r="K37" t="s">
+      <c r="M37" s="2">
+        <f t="shared" si="0"/>
+        <v>13.020000000000001</v>
+      </c>
+      <c r="N37" t="s">
         <v>85</v>
       </c>
-      <c r="L37" t="s">
+      <c r="O37" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>21</v>
       </c>
@@ -2227,22 +2405,32 @@
         <v>1.05</v>
       </c>
       <c r="H38" s="2">
+        <v>0.41</v>
+      </c>
+      <c r="I38" s="2">
+        <v>0.26040000000000002</v>
+      </c>
+      <c r="J38" s="2">
         <v>7.35</v>
       </c>
-      <c r="I38" s="2">
+      <c r="K38" s="2">
         <v>22.05</v>
       </c>
-      <c r="J38" s="2">
+      <c r="L38" s="2">
         <v>52.5</v>
       </c>
-      <c r="K38" t="s">
+      <c r="M38" s="2">
+        <f t="shared" si="0"/>
+        <v>13.020000000000001</v>
+      </c>
+      <c r="N38" t="s">
         <v>89</v>
       </c>
-      <c r="L38" t="s">
+      <c r="O38" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
       <c r="C39">
         <v>0</v>
       </c>
@@ -2250,17 +2438,23 @@
         <v>91</v>
       </c>
       <c r="G39" s="2"/>
-      <c r="H39" s="2">
-        <v>0</v>
-      </c>
-      <c r="I39" s="2">
-        <v>0</v>
-      </c>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
       <c r="J39" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K39" s="2">
+        <v>0</v>
+      </c>
+      <c r="L39" s="2">
+        <v>0</v>
+      </c>
+      <c r="M39" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>22</v>
       </c>
@@ -2280,23 +2474,29 @@
         <v>93</v>
       </c>
       <c r="G40" s="2"/>
-      <c r="H40" s="2">
-        <v>0</v>
-      </c>
-      <c r="I40" s="2">
-        <v>0</v>
-      </c>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
       <c r="J40" s="2">
         <v>0</v>
       </c>
-      <c r="K40" t="s">
+      <c r="K40" s="2">
+        <v>0</v>
+      </c>
+      <c r="L40" s="2">
+        <v>0</v>
+      </c>
+      <c r="M40" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N40" t="s">
         <v>94</v>
       </c>
-      <c r="L40" t="s">
+      <c r="O40" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>23</v>
       </c>
@@ -2316,17 +2516,23 @@
         <v>97</v>
       </c>
       <c r="G41" s="2"/>
-      <c r="H41" s="2">
-        <v>0</v>
-      </c>
-      <c r="I41" s="2">
-        <v>0</v>
-      </c>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
       <c r="J41" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K41" s="2">
+        <v>0</v>
+      </c>
+      <c r="L41" s="2">
+        <v>0</v>
+      </c>
+      <c r="M41" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>24</v>
       </c>
@@ -2349,22 +2555,32 @@
         <v>1.05</v>
       </c>
       <c r="H42" s="2">
+        <v>0.41</v>
+      </c>
+      <c r="I42" s="2">
+        <v>0.26040000000000002</v>
+      </c>
+      <c r="J42" s="2">
         <v>2.1</v>
       </c>
-      <c r="I42" s="2">
+      <c r="K42" s="2">
         <v>6.3</v>
       </c>
-      <c r="J42" s="2">
+      <c r="L42" s="2">
         <v>10.5</v>
       </c>
-      <c r="K42" t="s">
+      <c r="M42" s="2">
+        <f t="shared" si="0"/>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N42" t="s">
         <v>100</v>
       </c>
-      <c r="L42" t="s">
+      <c r="O42" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>25</v>
       </c>
@@ -2386,23 +2602,29 @@
       <c r="G43" s="2">
         <v>2.1</v>
       </c>
-      <c r="H43" s="2">
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2">
         <v>2.1</v>
       </c>
-      <c r="I43" s="2">
+      <c r="K43" s="2">
         <v>6.3</v>
       </c>
-      <c r="J43" s="2">
+      <c r="L43" s="2">
         <v>8.4</v>
       </c>
-      <c r="K43" t="s">
+      <c r="M43" s="2">
+        <f t="shared" si="0"/>
+        <v>8.4</v>
+      </c>
+      <c r="N43" t="s">
         <v>103</v>
       </c>
-      <c r="L43" t="s">
+      <c r="O43" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>26</v>
       </c>
@@ -2422,20 +2644,26 @@
         <v>106</v>
       </c>
       <c r="G44" s="2"/>
-      <c r="H44" s="2">
-        <v>0</v>
-      </c>
-      <c r="I44" s="2">
-        <v>0</v>
-      </c>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
       <c r="J44" s="2">
         <v>0</v>
       </c>
-      <c r="K44" t="s">
+      <c r="K44" s="2">
+        <v>0</v>
+      </c>
+      <c r="L44" s="2">
+        <v>0</v>
+      </c>
+      <c r="M44" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N44" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>27</v>
       </c>
@@ -2457,23 +2685,29 @@
       <c r="G45" s="2">
         <v>2.84</v>
       </c>
-      <c r="H45" s="2">
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2">
         <v>2.84</v>
       </c>
-      <c r="I45" s="2">
+      <c r="K45" s="2">
         <v>8.52</v>
       </c>
-      <c r="J45" s="2">
+      <c r="L45" s="2">
         <v>11.36</v>
       </c>
-      <c r="K45" t="s">
+      <c r="M45" s="2">
+        <f t="shared" si="0"/>
+        <v>11.36</v>
+      </c>
+      <c r="N45" t="s">
         <v>108</v>
       </c>
-      <c r="L45" t="s">
+      <c r="O45" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>28</v>
       </c>
@@ -2495,23 +2729,29 @@
       <c r="G46" s="2">
         <v>3.78</v>
       </c>
-      <c r="H46" s="2">
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2">
         <v>3.78</v>
       </c>
-      <c r="I46" s="2">
+      <c r="K46" s="2">
         <v>11.34</v>
       </c>
-      <c r="J46" s="2">
+      <c r="L46" s="2">
         <v>15.12</v>
       </c>
-      <c r="K46" t="s">
+      <c r="M46" s="2">
+        <f t="shared" si="0"/>
+        <v>15.12</v>
+      </c>
+      <c r="N46" t="s">
         <v>111</v>
       </c>
-      <c r="L46" t="s">
+      <c r="O46" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>29</v>
       </c>
@@ -2534,22 +2774,30 @@
         <v>3.47</v>
       </c>
       <c r="H47" s="2">
+        <v>2.3210000000000002</v>
+      </c>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2">
         <v>6.94</v>
       </c>
-      <c r="I47" s="2">
+      <c r="K47" s="2">
         <v>20.82</v>
       </c>
-      <c r="J47" s="2">
+      <c r="L47" s="2">
         <v>34.700000000000003</v>
       </c>
-      <c r="K47" t="s">
+      <c r="M47" s="2">
+        <f t="shared" si="0"/>
+        <v>23.21</v>
+      </c>
+      <c r="N47" t="s">
         <v>115</v>
       </c>
-      <c r="L47" t="s">
+      <c r="O47" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>30</v>
       </c>
@@ -2568,26 +2816,32 @@
       <c r="G48" s="2">
         <v>12.6</v>
       </c>
-      <c r="H48" s="2">
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2">
         <f>G48*B48</f>
         <v>12.6</v>
       </c>
-      <c r="I48" s="2">
+      <c r="K48" s="2">
         <f>G48*C48</f>
         <v>37.799999999999997</v>
       </c>
-      <c r="J48" s="2">
+      <c r="L48" s="2">
         <f>G48*D48</f>
         <v>50.4</v>
       </c>
-      <c r="K48" s="1" t="s">
+      <c r="M48" s="2">
+        <f t="shared" si="0"/>
+        <v>50.4</v>
+      </c>
+      <c r="N48" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="L48" t="s">
+      <c r="O48" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B49">
         <v>69</v>
       </c>
@@ -2597,20 +2851,26 @@
       <c r="G49" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="H49" s="2">
-        <f>SUM(H15:H48)</f>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2">
+        <f>SUM(J15:J48)</f>
         <v>222.51999999999995</v>
       </c>
-      <c r="I49" s="2">
-        <f>SUM(I15:I48)</f>
+      <c r="K49" s="2">
+        <f>SUM(K15:K48)</f>
         <v>667.55999999999983</v>
       </c>
-      <c r="J49" s="3">
-        <f>SUM(J15:J48)</f>
+      <c r="L49" s="3">
+        <f>SUM(L15:L48)</f>
         <v>939.61</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M49" s="3">
+        <f>SUM(M15:M48)</f>
+        <v>795.81999999999994</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B51" s="4" t="s">
         <v>118</v>
       </c>
@@ -2624,8 +2884,11 @@
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
       <c r="L51" s="4"/>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M51" s="4"/>
+      <c r="N51" s="4"/>
+      <c r="O51" s="4"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>31</v>
       </c>
@@ -2644,23 +2907,26 @@
       <c r="G52" s="2">
         <v>5.99</v>
       </c>
-      <c r="H52" s="2">
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2">
         <f>G52*B52</f>
         <v>5.99</v>
       </c>
-      <c r="I52" s="2">
+      <c r="K52" s="2">
         <f>G52*C52</f>
         <v>11.98</v>
       </c>
-      <c r="J52" s="2">
+      <c r="L52" s="2">
         <f>G52*D52</f>
         <v>11.98</v>
       </c>
-      <c r="L52" t="s">
+      <c r="M52" s="2"/>
+      <c r="O52" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>32</v>
       </c>
@@ -2679,23 +2945,26 @@
       <c r="G53" s="2">
         <v>7.98</v>
       </c>
-      <c r="H53" s="2">
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2">
         <f>G53*B53</f>
         <v>7.98</v>
       </c>
-      <c r="I53" s="2">
-        <f t="shared" ref="I53" si="0">G53*C53</f>
+      <c r="K53" s="2">
+        <f t="shared" ref="K53" si="1">G53*C53</f>
         <v>15.96</v>
       </c>
-      <c r="J53" s="2">
-        <f t="shared" ref="J53" si="1">G53*D53</f>
+      <c r="L53" s="2">
+        <f t="shared" ref="L53" si="2">G53*D53</f>
         <v>15.96</v>
       </c>
-      <c r="L53" t="s">
+      <c r="M53" s="2"/>
+      <c r="O53" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>33</v>
       </c>
@@ -2714,32 +2983,37 @@
       <c r="G54" s="2">
         <v>3.89</v>
       </c>
-      <c r="H54" s="2">
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2">
         <f>G54*B54</f>
         <v>3.89</v>
       </c>
-      <c r="I54" s="2">
-        <f t="shared" ref="I54" si="2">G54*C54</f>
+      <c r="K54" s="2">
+        <f t="shared" ref="K54" si="3">G54*C54</f>
         <v>11.67</v>
       </c>
-      <c r="J54" s="2">
-        <f t="shared" ref="J54" si="3">G54*D54</f>
+      <c r="L54" s="2">
+        <f t="shared" ref="L54" si="4">G54*D54</f>
         <v>11.67</v>
       </c>
-      <c r="L54" t="s">
+      <c r="M54" s="2"/>
+      <c r="O54" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="J55" s="2">
-        <f>SUM(J52:J54)</f>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="L55" s="2">
+        <f>SUM(L52:L54)</f>
         <v>39.61</v>
       </c>
+      <c r="M55" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B51:L51"/>
+    <mergeCell ref="B51:O51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added all components and expanded on pricing
</commit_message>
<xml_diff>
--- a/PCB-Node1/BOM_BYGGERNNODE1.xlsx
+++ b/PCB-Node1/BOM_BYGGERNNODE1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benja\Documents\Byggeren\TTK4155_Ping_Pong_Project\PCB-Node1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2211120-BBFF-433A-80C4-2932D5698227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{552B2BD7-DD45-45A7-B2A9-827AFD833DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{17AFD791-CEED-4828-96C0-A0F19B8C3E72}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="143">
   <si>
     <t>Byggern 2024 Node 1   Revised: Monday, October 21, 2024</t>
   </si>
@@ -441,6 +441,27 @@
   </si>
   <si>
     <t>Order cost</t>
+  </si>
+  <si>
+    <t>2 PCB Qantity</t>
+  </si>
+  <si>
+    <t>2 Board cost</t>
+  </si>
+  <si>
+    <t>1 Order cost</t>
+  </si>
+  <si>
+    <t>2 Order cost</t>
+  </si>
+  <si>
+    <t>parts Total:</t>
+  </si>
+  <si>
+    <t>3 Order cost</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -942,7 +963,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -950,6 +971,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -995,7 +1017,25 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="2" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="2" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1325,37 +1365,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D679CB1F-3136-4EF7-BB0E-65C07665A41B}">
-  <dimension ref="A1:O55"/>
+  <dimension ref="A1:T57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B48" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="A10" sqref="A10"/>
+      <selection pane="topRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomRight" activeCell="Q57" sqref="Q57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.90625" customWidth="1"/>
-    <col min="10" max="10" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="33.6328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="90" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.90625" customWidth="1"/>
+    <col min="11" max="12" width="17.453125" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="11.26953125" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="33.6328125" hidden="1" customWidth="1"/>
+    <col min="15" max="16" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.7265625" customWidth="1"/>
+    <col min="18" max="18" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="90" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1363,7 +1411,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1371,51 +1419,66 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
+        <v>136</v>
+      </c>
+      <c r="D12" t="s">
         <v>6</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>7</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>8</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>9</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>10</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>133</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>134</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>11</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
+        <v>137</v>
+      </c>
+      <c r="M12" t="s">
         <v>12</v>
       </c>
-      <c r="L12" t="s">
+      <c r="N12" t="s">
         <v>13</v>
       </c>
-      <c r="M12" t="s">
+      <c r="O12" t="s">
+        <v>138</v>
+      </c>
+      <c r="P12" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>141</v>
+      </c>
+      <c r="R12" t="s">
         <v>135</v>
       </c>
-      <c r="N12" t="s">
+      <c r="S12" t="s">
         <v>14</v>
       </c>
-      <c r="O12" t="s">
+      <c r="T12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1423,43 +1486,66 @@
         <v>2</v>
       </c>
       <c r="C15">
+        <f>B15*2</f>
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <f>B15*3</f>
         <v>6</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>6</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>17</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>18</v>
       </c>
-      <c r="G15" s="2">
+      <c r="H15" s="2">
         <v>12.81</v>
       </c>
-      <c r="H15" s="2"/>
       <c r="I15" s="2"/>
-      <c r="J15" s="2">
+      <c r="J15" s="2"/>
+      <c r="K15" s="2">
+        <f>B15*H15</f>
         <v>25.62</v>
       </c>
-      <c r="K15" s="2">
+      <c r="L15" s="2">
+        <f>C15*H15</f>
+        <v>51.24</v>
+      </c>
+      <c r="M15" s="2">
         <v>76.86</v>
       </c>
-      <c r="L15" s="2">
+      <c r="N15" s="2">
+        <f>E15*H15</f>
         <v>76.86</v>
       </c>
-      <c r="M15" s="2">
-        <f>IF(D15&gt;=50,D15*I15,IF(D15&gt;=10,D15*H15,D15*G15))</f>
+      <c r="O15" s="2">
+        <f>IF(B15&gt;=50,B15*J15,IF(B15&gt;=10,B15*I15,B15*H15))</f>
+        <v>25.62</v>
+      </c>
+      <c r="P15" s="2">
+        <f>IF(C15&gt;=50,C15*J15,IF(C15&gt;=10,C15*I15,C15*H15))</f>
+        <v>51.24</v>
+      </c>
+      <c r="Q15" s="2">
+        <f>IF(D15&gt;=50,D15*J15,IF(D15&gt;=10,D15*I15,D15*H15))</f>
         <v>76.86</v>
       </c>
-      <c r="N15" s="1" t="s">
+      <c r="R15" s="2">
+        <f>IF(E15&gt;=50,E15*J15,IF(E15&gt;=10,E15*I15,E15*H15))</f>
+        <v>76.86</v>
+      </c>
+      <c r="S15" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="O15" t="s">
+      <c r="T15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1467,43 +1553,66 @@
         <v>1</v>
       </c>
       <c r="C16">
+        <f t="shared" ref="C16:C48" si="0">B16*2</f>
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ref="D16:D48" si="1">B16*3</f>
         <v>3</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>5</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>20</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>865080457015</v>
       </c>
-      <c r="G16" s="2">
+      <c r="H16" s="2">
         <v>10.19</v>
       </c>
-      <c r="H16" s="2"/>
       <c r="I16" s="2"/>
-      <c r="J16" s="2">
+      <c r="J16" s="2"/>
+      <c r="K16" s="2">
+        <f t="shared" ref="K16:K48" si="2">B16*H16</f>
         <v>10.19</v>
       </c>
-      <c r="K16" s="2">
+      <c r="L16" s="2">
+        <f t="shared" ref="L16:L48" si="3">C16*H16</f>
+        <v>20.38</v>
+      </c>
+      <c r="M16" s="2">
         <v>30.57</v>
       </c>
-      <c r="L16" s="2">
-        <v>50.95</v>
-      </c>
-      <c r="M16" s="2">
-        <f t="shared" ref="M16:M48" si="0">IF(D16&gt;=50,D16*I16,IF(D16&gt;=10,D16*H16,D16*G16))</f>
+      <c r="N16" s="2">
+        <f t="shared" ref="N16:N48" si="4">E16*H16</f>
         <v>50.949999999999996</v>
       </c>
-      <c r="N16" s="1" t="s">
+      <c r="O16" s="2">
+        <f t="shared" ref="O16:O48" si="5">IF(B16&gt;=50,B16*J16,IF(B16&gt;=10,B16*I16,B16*H16))</f>
+        <v>10.19</v>
+      </c>
+      <c r="P16" s="2">
+        <f t="shared" ref="P16:P48" si="6">IF(C16&gt;=50,C16*J16,IF(C16&gt;=10,C16*I16,C16*H16))</f>
+        <v>20.38</v>
+      </c>
+      <c r="Q16" s="2">
+        <f t="shared" ref="Q16:Q49" si="7">IF(D16&gt;=50,D16*J16,IF(D16&gt;=10,D16*I16,D16*H16))</f>
+        <v>30.57</v>
+      </c>
+      <c r="R16" s="2">
+        <f t="shared" ref="R16:R48" si="8">IF(E16&gt;=50,E16*J16,IF(E16&gt;=10,E16*I16,E16*H16))</f>
+        <v>50.949999999999996</v>
+      </c>
+      <c r="S16" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="O16" t="s">
+      <c r="T16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>3</v>
       </c>
@@ -1511,211 +1620,349 @@
         <v>1</v>
       </c>
       <c r="C17">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>5</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>22</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>865080253012</v>
       </c>
-      <c r="G17" s="2">
+      <c r="H17" s="2">
         <v>5.99</v>
       </c>
-      <c r="H17" s="2"/>
       <c r="I17" s="2"/>
-      <c r="J17" s="2">
+      <c r="J17" s="2"/>
+      <c r="K17" s="2">
+        <f t="shared" si="2"/>
         <v>5.99</v>
       </c>
-      <c r="K17" s="2">
+      <c r="L17" s="2">
+        <f t="shared" si="3"/>
+        <v>11.98</v>
+      </c>
+      <c r="M17" s="2">
         <v>17.97</v>
       </c>
-      <c r="L17" s="2">
-        <v>29.95</v>
-      </c>
-      <c r="M17" s="2">
-        <f t="shared" si="0"/>
+      <c r="N17" s="2">
+        <f t="shared" si="4"/>
         <v>29.950000000000003</v>
       </c>
-      <c r="N17" s="1" t="s">
+      <c r="O17" s="2">
+        <f t="shared" si="5"/>
+        <v>5.99</v>
+      </c>
+      <c r="P17" s="2">
+        <f t="shared" si="6"/>
+        <v>11.98</v>
+      </c>
+      <c r="Q17" s="2">
+        <f t="shared" si="7"/>
+        <v>17.97</v>
+      </c>
+      <c r="R17" s="2">
+        <f t="shared" si="8"/>
+        <v>29.950000000000003</v>
+      </c>
+      <c r="S17" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="O17" t="s">
+      <c r="T17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>4</v>
       </c>
       <c r="B18">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C18">
-        <v>45</v>
+        <f t="shared" si="0"/>
+        <v>34</v>
       </c>
       <c r="D18">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="E18">
         <v>50</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>24</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="2">
+      <c r="H18" s="2">
         <v>2</v>
-      </c>
-      <c r="H18" s="2">
-        <v>1.859</v>
       </c>
       <c r="I18" s="2">
         <v>1.859</v>
       </c>
       <c r="J18" s="2">
-        <v>30</v>
+        <v>1.859</v>
       </c>
       <c r="K18" s="2">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="L18" s="2">
+        <f t="shared" si="3"/>
+        <v>68</v>
+      </c>
+      <c r="M18" s="2">
         <v>90</v>
       </c>
-      <c r="L18" s="2">
+      <c r="N18" s="2">
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
-      <c r="M18" s="2">
+      <c r="O18" s="2">
+        <f t="shared" si="5"/>
+        <v>31.603000000000002</v>
+      </c>
+      <c r="P18" s="2">
+        <f t="shared" si="6"/>
+        <v>63.206000000000003</v>
+      </c>
+      <c r="Q18" s="2">
+        <f t="shared" si="7"/>
+        <v>94.808999999999997</v>
+      </c>
+      <c r="R18" s="2">
+        <f t="shared" si="8"/>
+        <v>92.95</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="T18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="C19">
         <f t="shared" si="0"/>
-        <v>92.95</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="O18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="E19" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F19" t="s">
         <v>27</v>
       </c>
-      <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
-      <c r="J19" s="2">
-        <v>0</v>
-      </c>
+      <c r="J19" s="2"/>
       <c r="K19" s="2">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L19" s="2">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M19" s="2">
+        <v>0</v>
+      </c>
+      <c r="N19" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O19" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P19" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q19" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="R19" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="C20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
         <v>28</v>
       </c>
-      <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
-      <c r="J20" s="2">
-        <v>0</v>
-      </c>
+      <c r="J20" s="2"/>
       <c r="K20" s="2">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L20" s="2">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M20" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="N20" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O20" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P20" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q20" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="R20" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>5</v>
       </c>
       <c r="B21">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C21">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="E21">
+        <v>50</v>
+      </c>
+      <c r="F21" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" t="s">
+        <v>30</v>
+      </c>
+      <c r="H21" s="2">
+        <v>1.26</v>
+      </c>
+      <c r="I21" s="2">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="J21" s="2">
+        <v>0.50619999999999998</v>
+      </c>
+      <c r="K21" s="2">
+        <f t="shared" si="2"/>
+        <v>15.120000000000001</v>
+      </c>
+      <c r="L21" s="2">
+        <f t="shared" si="3"/>
+        <v>30.240000000000002</v>
+      </c>
+      <c r="M21" s="2">
+        <v>41.58</v>
+      </c>
+      <c r="N21" s="2">
+        <f t="shared" si="4"/>
+        <v>63</v>
+      </c>
+      <c r="O21" s="2">
+        <f t="shared" si="5"/>
+        <v>8.82</v>
+      </c>
+      <c r="P21" s="2">
+        <f t="shared" si="6"/>
+        <v>17.64</v>
+      </c>
+      <c r="Q21" s="2">
+        <f t="shared" si="7"/>
+        <v>26.46</v>
+      </c>
+      <c r="R21" s="2">
+        <f t="shared" si="8"/>
+        <v>25.31</v>
+      </c>
+      <c r="S21" t="s">
+        <v>31</v>
+      </c>
+      <c r="T21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F22" t="s">
         <v>33</v>
       </c>
-      <c r="D21">
-        <v>50</v>
-      </c>
-      <c r="E21" t="s">
-        <v>29</v>
-      </c>
-      <c r="F21" t="s">
-        <v>30</v>
-      </c>
-      <c r="G21" s="2">
-        <v>1.26</v>
-      </c>
-      <c r="H21" s="2">
-        <v>0.73499999999999999</v>
-      </c>
-      <c r="I21" s="2">
-        <v>0.50619999999999998</v>
-      </c>
-      <c r="J21" s="2">
-        <v>13.86</v>
-      </c>
-      <c r="K21" s="2">
-        <v>41.58</v>
-      </c>
-      <c r="L21" s="2">
-        <v>63</v>
-      </c>
-      <c r="M21" s="2">
-        <f t="shared" si="0"/>
-        <v>25.31</v>
-      </c>
-      <c r="N21" t="s">
-        <v>31</v>
-      </c>
-      <c r="O21" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="E22" t="s">
-        <v>33</v>
-      </c>
-      <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
-      <c r="J22" s="2">
-        <v>0</v>
-      </c>
+      <c r="J22" s="2"/>
       <c r="K22" s="2">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L22" s="2">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M22" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="N22" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O22" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P22" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q22" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="R22" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>6</v>
       </c>
@@ -1723,47 +1970,70 @@
         <v>2</v>
       </c>
       <c r="C23">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>10</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>34</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>35</v>
       </c>
-      <c r="G23" s="2">
+      <c r="H23" s="2">
         <v>1.05</v>
-      </c>
-      <c r="H23" s="2">
-        <v>0.83</v>
       </c>
       <c r="I23" s="2">
         <v>0.83</v>
       </c>
       <c r="J23" s="2">
+        <v>0.83</v>
+      </c>
+      <c r="K23" s="2">
+        <f t="shared" si="2"/>
         <v>2.1</v>
       </c>
-      <c r="K23" s="2">
+      <c r="L23" s="2">
+        <f t="shared" si="3"/>
+        <v>4.2</v>
+      </c>
+      <c r="M23" s="2">
         <v>6.3</v>
       </c>
-      <c r="L23" s="2">
+      <c r="N23" s="2">
+        <f t="shared" si="4"/>
         <v>10.5</v>
       </c>
-      <c r="M23" s="2">
-        <f t="shared" si="0"/>
+      <c r="O23" s="2">
+        <f t="shared" si="5"/>
+        <v>2.1</v>
+      </c>
+      <c r="P23" s="2">
+        <f t="shared" si="6"/>
+        <v>4.2</v>
+      </c>
+      <c r="Q23" s="2">
+        <f t="shared" si="7"/>
+        <v>6.3000000000000007</v>
+      </c>
+      <c r="R23" s="2">
+        <f t="shared" si="8"/>
         <v>8.2999999999999989</v>
       </c>
-      <c r="N23" s="1" t="s">
+      <c r="S23" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="O23" t="s">
+      <c r="T23" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>7</v>
       </c>
@@ -1771,43 +2041,66 @@
         <v>1</v>
       </c>
       <c r="C24">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>4</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>37</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>38</v>
       </c>
-      <c r="G24" s="2">
+      <c r="H24" s="2">
         <v>11.55</v>
       </c>
-      <c r="H24" s="2"/>
       <c r="I24" s="2"/>
-      <c r="J24" s="2">
+      <c r="J24" s="2"/>
+      <c r="K24" s="2">
+        <f t="shared" si="2"/>
         <v>11.55</v>
       </c>
-      <c r="K24" s="2">
+      <c r="L24" s="2">
+        <f t="shared" si="3"/>
+        <v>23.1</v>
+      </c>
+      <c r="M24" s="2">
         <v>34.65</v>
       </c>
-      <c r="L24" s="2">
+      <c r="N24" s="2">
+        <f t="shared" si="4"/>
         <v>46.2</v>
       </c>
-      <c r="M24" s="2">
-        <f t="shared" si="0"/>
+      <c r="O24" s="2">
+        <f t="shared" si="5"/>
+        <v>11.55</v>
+      </c>
+      <c r="P24" s="2">
+        <f t="shared" si="6"/>
+        <v>23.1</v>
+      </c>
+      <c r="Q24" s="2">
+        <f t="shared" si="7"/>
+        <v>34.650000000000006</v>
+      </c>
+      <c r="R24" s="2">
+        <f t="shared" si="8"/>
         <v>46.2</v>
       </c>
-      <c r="N24" t="s">
+      <c r="S24" t="s">
         <v>39</v>
       </c>
-      <c r="O24" t="s">
+      <c r="T24" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>8</v>
       </c>
@@ -1815,43 +2108,66 @@
         <v>1</v>
       </c>
       <c r="C25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>4</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>41</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>42</v>
       </c>
-      <c r="G25" s="2">
+      <c r="H25" s="2">
         <v>4.0999999999999996</v>
       </c>
-      <c r="H25" s="2"/>
       <c r="I25" s="2"/>
-      <c r="J25" s="2">
+      <c r="J25" s="2"/>
+      <c r="K25" s="2">
+        <f t="shared" si="2"/>
         <v>4.0999999999999996</v>
       </c>
-      <c r="K25" s="2">
+      <c r="L25" s="2">
+        <f t="shared" si="3"/>
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="M25" s="2">
         <v>12.3</v>
       </c>
-      <c r="L25" s="2">
+      <c r="N25" s="2">
+        <f t="shared" si="4"/>
         <v>16.399999999999999</v>
       </c>
-      <c r="M25" s="2">
-        <f t="shared" si="0"/>
+      <c r="O25" s="2">
+        <f t="shared" si="5"/>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="P25" s="2">
+        <f t="shared" si="6"/>
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="Q25" s="2">
+        <f t="shared" si="7"/>
+        <v>12.299999999999999</v>
+      </c>
+      <c r="R25" s="2">
+        <f t="shared" si="8"/>
         <v>16.399999999999999</v>
       </c>
-      <c r="N25" t="s">
+      <c r="S25" t="s">
         <v>43</v>
       </c>
-      <c r="O25" t="s">
+      <c r="T25" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>9</v>
       </c>
@@ -1859,43 +2175,66 @@
         <v>1</v>
       </c>
       <c r="C26">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>4</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>45</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>46</v>
       </c>
-      <c r="G26" s="2">
+      <c r="H26" s="2">
         <v>5.78</v>
       </c>
-      <c r="H26" s="2"/>
       <c r="I26" s="2"/>
-      <c r="J26" s="2">
+      <c r="J26" s="2"/>
+      <c r="K26" s="2">
+        <f t="shared" si="2"/>
         <v>5.78</v>
       </c>
-      <c r="K26" s="2">
+      <c r="L26" s="2">
+        <f t="shared" si="3"/>
+        <v>11.56</v>
+      </c>
+      <c r="M26" s="2">
         <v>17.34</v>
       </c>
-      <c r="L26" s="2">
+      <c r="N26" s="2">
+        <f t="shared" si="4"/>
         <v>23.12</v>
       </c>
-      <c r="M26" s="2">
-        <f t="shared" si="0"/>
+      <c r="O26" s="2">
+        <f t="shared" si="5"/>
+        <v>5.78</v>
+      </c>
+      <c r="P26" s="2">
+        <f t="shared" si="6"/>
+        <v>11.56</v>
+      </c>
+      <c r="Q26" s="2">
+        <f t="shared" si="7"/>
+        <v>17.34</v>
+      </c>
+      <c r="R26" s="2">
+        <f t="shared" si="8"/>
         <v>23.12</v>
       </c>
-      <c r="N26" t="s">
+      <c r="S26" t="s">
         <v>47</v>
       </c>
-      <c r="O26" t="s">
+      <c r="T26" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>10</v>
       </c>
@@ -1903,43 +2242,66 @@
         <v>1</v>
       </c>
       <c r="C27">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="D27">
+      <c r="E27">
         <v>4</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>49</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>50</v>
       </c>
-      <c r="G27" s="2">
+      <c r="H27" s="2">
         <v>5.88</v>
       </c>
-      <c r="H27" s="2"/>
       <c r="I27" s="2"/>
-      <c r="J27" s="2">
+      <c r="J27" s="2"/>
+      <c r="K27" s="2">
+        <f t="shared" si="2"/>
         <v>5.88</v>
       </c>
-      <c r="K27" s="2">
+      <c r="L27" s="2">
+        <f t="shared" si="3"/>
+        <v>11.76</v>
+      </c>
+      <c r="M27" s="2">
         <v>17.64</v>
       </c>
-      <c r="L27" s="2">
+      <c r="N27" s="2">
+        <f t="shared" si="4"/>
         <v>23.52</v>
       </c>
-      <c r="M27" s="2">
-        <f t="shared" si="0"/>
+      <c r="O27" s="2">
+        <f t="shared" si="5"/>
+        <v>5.88</v>
+      </c>
+      <c r="P27" s="2">
+        <f t="shared" si="6"/>
+        <v>11.76</v>
+      </c>
+      <c r="Q27" s="2">
+        <f t="shared" si="7"/>
+        <v>17.64</v>
+      </c>
+      <c r="R27" s="2">
+        <f t="shared" si="8"/>
         <v>23.52</v>
       </c>
-      <c r="N27" t="s">
+      <c r="S27" t="s">
         <v>51</v>
       </c>
-      <c r="O27" t="s">
+      <c r="T27" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>11</v>
       </c>
@@ -1947,43 +2309,66 @@
         <v>1</v>
       </c>
       <c r="C28">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <v>4</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>53</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>54</v>
       </c>
-      <c r="G28" s="2">
+      <c r="H28" s="2">
         <v>5.57</v>
       </c>
-      <c r="H28" s="2"/>
       <c r="I28" s="2"/>
-      <c r="J28" s="2">
+      <c r="J28" s="2"/>
+      <c r="K28" s="2">
+        <f t="shared" si="2"/>
         <v>5.57</v>
       </c>
-      <c r="K28" s="2">
+      <c r="L28" s="2">
+        <f t="shared" si="3"/>
+        <v>11.14</v>
+      </c>
+      <c r="M28" s="2">
         <v>16.71</v>
       </c>
-      <c r="L28" s="2">
+      <c r="N28" s="2">
+        <f t="shared" si="4"/>
         <v>22.28</v>
       </c>
-      <c r="M28" s="2">
-        <f t="shared" si="0"/>
+      <c r="O28" s="2">
+        <f t="shared" si="5"/>
+        <v>5.57</v>
+      </c>
+      <c r="P28" s="2">
+        <f t="shared" si="6"/>
+        <v>11.14</v>
+      </c>
+      <c r="Q28" s="2">
+        <f t="shared" si="7"/>
+        <v>16.71</v>
+      </c>
+      <c r="R28" s="2">
+        <f t="shared" si="8"/>
         <v>22.28</v>
       </c>
-      <c r="N28" t="s">
+      <c r="S28" t="s">
         <v>55</v>
       </c>
-      <c r="O28" t="s">
+      <c r="T28" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>12</v>
       </c>
@@ -1991,43 +2376,66 @@
         <v>1</v>
       </c>
       <c r="C29">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="D29">
+      <c r="E29">
         <v>4</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>57</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>58</v>
       </c>
-      <c r="G29" s="2">
+      <c r="H29" s="2">
         <v>3.99</v>
       </c>
-      <c r="H29" s="2"/>
       <c r="I29" s="2"/>
-      <c r="J29" s="2">
+      <c r="J29" s="2"/>
+      <c r="K29" s="2">
+        <f t="shared" si="2"/>
         <v>3.99</v>
       </c>
-      <c r="K29" s="2">
+      <c r="L29" s="2">
+        <f t="shared" si="3"/>
+        <v>7.98</v>
+      </c>
+      <c r="M29" s="2">
         <v>11.97</v>
       </c>
-      <c r="L29" s="2">
+      <c r="N29" s="2">
+        <f t="shared" si="4"/>
         <v>15.96</v>
       </c>
-      <c r="M29" s="2">
-        <f t="shared" si="0"/>
+      <c r="O29" s="2">
+        <f t="shared" si="5"/>
+        <v>3.99</v>
+      </c>
+      <c r="P29" s="2">
+        <f t="shared" si="6"/>
+        <v>7.98</v>
+      </c>
+      <c r="Q29" s="2">
+        <f t="shared" si="7"/>
+        <v>11.97</v>
+      </c>
+      <c r="R29" s="2">
+        <f t="shared" si="8"/>
         <v>15.96</v>
       </c>
-      <c r="N29" t="s">
+      <c r="S29" t="s">
         <v>59</v>
       </c>
-      <c r="O29" t="s">
+      <c r="T29" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>13</v>
       </c>
@@ -2035,43 +2443,66 @@
         <v>1</v>
       </c>
       <c r="C30">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="D30">
+      <c r="E30">
         <v>4</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>61</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>62</v>
       </c>
-      <c r="G30" s="2">
+      <c r="H30" s="2">
         <v>3.26</v>
       </c>
-      <c r="H30" s="2"/>
       <c r="I30" s="2"/>
-      <c r="J30" s="2">
+      <c r="J30" s="2"/>
+      <c r="K30" s="2">
+        <f t="shared" si="2"/>
         <v>3.26</v>
       </c>
-      <c r="K30" s="2">
+      <c r="L30" s="2">
+        <f t="shared" si="3"/>
+        <v>6.52</v>
+      </c>
+      <c r="M30" s="2">
         <v>9.7799999999999994</v>
       </c>
-      <c r="L30" s="2">
+      <c r="N30" s="2">
+        <f t="shared" si="4"/>
         <v>13.04</v>
       </c>
-      <c r="M30" s="2">
-        <f t="shared" si="0"/>
+      <c r="O30" s="2">
+        <f t="shared" si="5"/>
+        <v>3.26</v>
+      </c>
+      <c r="P30" s="2">
+        <f t="shared" si="6"/>
+        <v>6.52</v>
+      </c>
+      <c r="Q30" s="2">
+        <f t="shared" si="7"/>
+        <v>9.7799999999999994</v>
+      </c>
+      <c r="R30" s="2">
+        <f t="shared" si="8"/>
         <v>13.04</v>
       </c>
-      <c r="N30" t="s">
+      <c r="S30" t="s">
         <v>63</v>
       </c>
-      <c r="O30" t="s">
+      <c r="T30" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>14</v>
       </c>
@@ -2079,43 +2510,66 @@
         <v>1</v>
       </c>
       <c r="C31">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="D31">
+      <c r="E31">
         <v>4</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>65</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>66</v>
       </c>
-      <c r="G31" s="2">
+      <c r="H31" s="2">
         <v>12.39</v>
       </c>
-      <c r="H31" s="2"/>
       <c r="I31" s="2"/>
-      <c r="J31" s="2">
+      <c r="J31" s="2"/>
+      <c r="K31" s="2">
+        <f t="shared" si="2"/>
         <v>12.39</v>
       </c>
-      <c r="K31" s="2">
+      <c r="L31" s="2">
+        <f t="shared" si="3"/>
+        <v>24.78</v>
+      </c>
+      <c r="M31" s="2">
         <v>37.17</v>
       </c>
-      <c r="L31" s="2">
+      <c r="N31" s="2">
+        <f t="shared" si="4"/>
         <v>49.56</v>
       </c>
-      <c r="M31" s="2">
-        <f t="shared" si="0"/>
+      <c r="O31" s="2">
+        <f t="shared" si="5"/>
+        <v>12.39</v>
+      </c>
+      <c r="P31" s="2">
+        <f t="shared" si="6"/>
+        <v>24.78</v>
+      </c>
+      <c r="Q31" s="2">
+        <f t="shared" si="7"/>
+        <v>37.17</v>
+      </c>
+      <c r="R31" s="2">
+        <f t="shared" si="8"/>
         <v>49.56</v>
       </c>
-      <c r="N31" t="s">
+      <c r="S31" t="s">
         <v>66</v>
       </c>
-      <c r="O31" t="s">
+      <c r="T31" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>15</v>
       </c>
@@ -2123,43 +2577,66 @@
         <v>1</v>
       </c>
       <c r="C32">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="D32">
+      <c r="E32">
         <v>4</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>68</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>69</v>
       </c>
-      <c r="G32" s="2">
+      <c r="H32" s="2">
         <v>11.55</v>
       </c>
-      <c r="H32" s="2"/>
       <c r="I32" s="2"/>
-      <c r="J32" s="2">
+      <c r="J32" s="2"/>
+      <c r="K32" s="2">
+        <f t="shared" si="2"/>
         <v>11.55</v>
       </c>
-      <c r="K32" s="2">
+      <c r="L32" s="2">
+        <f t="shared" si="3"/>
+        <v>23.1</v>
+      </c>
+      <c r="M32" s="2">
         <v>34.65</v>
       </c>
-      <c r="L32" s="2">
+      <c r="N32" s="2">
+        <f t="shared" si="4"/>
         <v>46.2</v>
       </c>
-      <c r="M32" s="2">
-        <f t="shared" si="0"/>
+      <c r="O32" s="2">
+        <f t="shared" si="5"/>
+        <v>11.55</v>
+      </c>
+      <c r="P32" s="2">
+        <f t="shared" si="6"/>
+        <v>23.1</v>
+      </c>
+      <c r="Q32" s="2">
+        <f t="shared" si="7"/>
+        <v>34.650000000000006</v>
+      </c>
+      <c r="R32" s="2">
+        <f t="shared" si="8"/>
         <v>46.2</v>
       </c>
-      <c r="N32" s="1" t="s">
+      <c r="S32" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="O32" t="s">
+      <c r="T32" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>16</v>
       </c>
@@ -2167,43 +2644,66 @@
         <v>1</v>
       </c>
       <c r="C33">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="D33">
+      <c r="E33">
         <v>4</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>71</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>72</v>
       </c>
-      <c r="G33" s="2">
+      <c r="H33" s="2">
         <v>17.12</v>
       </c>
-      <c r="H33" s="2"/>
       <c r="I33" s="2"/>
-      <c r="J33" s="2">
+      <c r="J33" s="2"/>
+      <c r="K33" s="2">
+        <f t="shared" si="2"/>
         <v>17.12</v>
       </c>
-      <c r="K33" s="2">
+      <c r="L33" s="2">
+        <f t="shared" si="3"/>
+        <v>34.24</v>
+      </c>
+      <c r="M33" s="2">
         <v>51.36</v>
       </c>
-      <c r="L33" s="2">
+      <c r="N33" s="2">
+        <f t="shared" si="4"/>
         <v>68.48</v>
       </c>
-      <c r="M33" s="2">
-        <f t="shared" si="0"/>
+      <c r="O33" s="2">
+        <f t="shared" si="5"/>
+        <v>17.12</v>
+      </c>
+      <c r="P33" s="2">
+        <f t="shared" si="6"/>
+        <v>34.24</v>
+      </c>
+      <c r="Q33" s="2">
+        <f t="shared" si="7"/>
+        <v>51.36</v>
+      </c>
+      <c r="R33" s="2">
+        <f t="shared" si="8"/>
         <v>68.48</v>
       </c>
-      <c r="N33" t="s">
+      <c r="S33" t="s">
         <v>72</v>
       </c>
-      <c r="O33" t="s">
+      <c r="T33" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>17</v>
       </c>
@@ -2211,43 +2711,66 @@
         <v>1</v>
       </c>
       <c r="C34">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="D34">
+      <c r="E34">
         <v>4</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>74</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>75</v>
       </c>
-      <c r="G34" s="2">
+      <c r="H34" s="2">
         <v>4.9400000000000004</v>
       </c>
-      <c r="H34" s="2"/>
       <c r="I34" s="2"/>
-      <c r="J34" s="2">
+      <c r="J34" s="2"/>
+      <c r="K34" s="2">
+        <f t="shared" si="2"/>
         <v>4.9400000000000004</v>
       </c>
-      <c r="K34" s="2">
+      <c r="L34" s="2">
+        <f t="shared" si="3"/>
+        <v>9.8800000000000008</v>
+      </c>
+      <c r="M34" s="2">
         <v>14.82</v>
       </c>
-      <c r="L34" s="2">
+      <c r="N34" s="2">
+        <f t="shared" si="4"/>
         <v>19.760000000000002</v>
       </c>
-      <c r="M34" s="2">
-        <f t="shared" si="0"/>
+      <c r="O34" s="2">
+        <f t="shared" si="5"/>
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="P34" s="2">
+        <f t="shared" si="6"/>
+        <v>9.8800000000000008</v>
+      </c>
+      <c r="Q34" s="2">
+        <f t="shared" si="7"/>
+        <v>14.82</v>
+      </c>
+      <c r="R34" s="2">
+        <f t="shared" si="8"/>
         <v>19.760000000000002</v>
       </c>
-      <c r="N34" t="s">
+      <c r="S34" t="s">
         <v>75</v>
       </c>
-      <c r="O34" t="s">
+      <c r="T34" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>18</v>
       </c>
@@ -2255,86 +2778,132 @@
         <v>3</v>
       </c>
       <c r="C35">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="D35">
+      <c r="E35">
         <v>15</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>77</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>78</v>
-      </c>
-      <c r="G35" s="2">
-        <v>1.89</v>
       </c>
       <c r="H35" s="2">
         <v>1.89</v>
       </c>
       <c r="I35" s="2">
+        <v>1.89</v>
+      </c>
+      <c r="J35" s="2">
         <v>1.8480000000000001</v>
       </c>
-      <c r="J35" s="2">
+      <c r="K35" s="2">
+        <f t="shared" si="2"/>
         <v>5.67</v>
       </c>
-      <c r="K35" s="2">
+      <c r="L35" s="2">
+        <f t="shared" si="3"/>
+        <v>11.34</v>
+      </c>
+      <c r="M35" s="2">
         <v>17.010000000000002</v>
       </c>
-      <c r="L35" s="2">
-        <v>28.35</v>
-      </c>
-      <c r="M35" s="2">
-        <f t="shared" si="0"/>
+      <c r="N35" s="2">
+        <f t="shared" si="4"/>
         <v>28.349999999999998</v>
       </c>
-      <c r="N35" t="s">
+      <c r="O35" s="2">
+        <f t="shared" si="5"/>
+        <v>5.67</v>
+      </c>
+      <c r="P35" s="2">
+        <f t="shared" si="6"/>
+        <v>11.34</v>
+      </c>
+      <c r="Q35" s="2">
+        <f t="shared" si="7"/>
+        <v>17.009999999999998</v>
+      </c>
+      <c r="R35" s="2">
+        <f t="shared" si="8"/>
+        <v>28.349999999999998</v>
+      </c>
+      <c r="S35" t="s">
         <v>78</v>
       </c>
-      <c r="O35" t="s">
+      <c r="T35" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>19</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C36">
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="D36">
-        <v>0</v>
-      </c>
-      <c r="E36" t="s">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36" t="s">
         <v>80</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>81</v>
       </c>
-      <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
-      <c r="J36" s="2">
-        <v>0</v>
-      </c>
+      <c r="J36" s="2"/>
       <c r="K36" s="2">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L36" s="2">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M36" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N36" t="s">
+        <v>0</v>
+      </c>
+      <c r="N36" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O36" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P36" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q36" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="R36" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="S36" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>20</v>
       </c>
@@ -2342,47 +2911,70 @@
         <v>5</v>
       </c>
       <c r="C37">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="D37">
+      <c r="E37">
         <v>50</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>83</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>84</v>
       </c>
-      <c r="G37" s="2">
+      <c r="H37" s="2">
         <v>1.05</v>
       </c>
-      <c r="H37" s="2">
+      <c r="I37" s="2">
         <v>0.41</v>
       </c>
-      <c r="I37" s="2">
+      <c r="J37" s="2">
         <v>0.26040000000000002</v>
       </c>
-      <c r="J37" s="2">
+      <c r="K37" s="2">
+        <f t="shared" si="2"/>
         <v>5.25</v>
       </c>
-      <c r="K37" s="2">
+      <c r="L37" s="2">
+        <f t="shared" si="3"/>
+        <v>10.5</v>
+      </c>
+      <c r="M37" s="2">
         <v>15.75</v>
       </c>
-      <c r="L37" s="2">
+      <c r="N37" s="2">
+        <f t="shared" si="4"/>
         <v>52.5</v>
       </c>
-      <c r="M37" s="2">
-        <f t="shared" si="0"/>
+      <c r="O37" s="2">
+        <f t="shared" si="5"/>
+        <v>5.25</v>
+      </c>
+      <c r="P37" s="2">
+        <f t="shared" si="6"/>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="Q37" s="2">
+        <f t="shared" si="7"/>
+        <v>6.1499999999999995</v>
+      </c>
+      <c r="R37" s="2">
+        <f t="shared" si="8"/>
         <v>13.020000000000001</v>
       </c>
-      <c r="N37" t="s">
+      <c r="S37" t="s">
         <v>85</v>
       </c>
-      <c r="O37" t="s">
+      <c r="T37" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>21</v>
       </c>
@@ -2390,149 +2982,245 @@
         <v>7</v>
       </c>
       <c r="C38">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="D38">
+      <c r="E38">
         <v>50</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>87</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>88</v>
       </c>
-      <c r="G38" s="2">
+      <c r="H38" s="2">
         <v>1.05</v>
       </c>
-      <c r="H38" s="2">
+      <c r="I38" s="2">
         <v>0.41</v>
       </c>
-      <c r="I38" s="2">
+      <c r="J38" s="2">
         <v>0.26040000000000002</v>
       </c>
-      <c r="J38" s="2">
-        <v>7.35</v>
-      </c>
       <c r="K38" s="2">
+        <f t="shared" si="2"/>
+        <v>7.3500000000000005</v>
+      </c>
+      <c r="L38" s="2">
+        <f t="shared" si="3"/>
+        <v>14.700000000000001</v>
+      </c>
+      <c r="M38" s="2">
         <v>22.05</v>
       </c>
-      <c r="L38" s="2">
+      <c r="N38" s="2">
+        <f t="shared" si="4"/>
         <v>52.5</v>
       </c>
-      <c r="M38" s="2">
+      <c r="O38" s="2">
+        <f t="shared" si="5"/>
+        <v>7.3500000000000005</v>
+      </c>
+      <c r="P38" s="2">
+        <f t="shared" si="6"/>
+        <v>5.7399999999999993</v>
+      </c>
+      <c r="Q38" s="2">
+        <f t="shared" si="7"/>
+        <v>8.61</v>
+      </c>
+      <c r="R38" s="2">
+        <f t="shared" si="8"/>
+        <v>13.020000000000001</v>
+      </c>
+      <c r="S38" t="s">
+        <v>89</v>
+      </c>
+      <c r="T38" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="C39">
         <f t="shared" si="0"/>
-        <v>13.020000000000001</v>
-      </c>
-      <c r="N38" t="s">
-        <v>89</v>
-      </c>
-      <c r="O38" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="C39">
-        <v>0</v>
-      </c>
-      <c r="E39" t="s">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F39" t="s">
         <v>91</v>
       </c>
-      <c r="G39" s="2"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
-      <c r="J39" s="2">
-        <v>0</v>
-      </c>
+      <c r="J39" s="2"/>
       <c r="K39" s="2">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L39" s="2">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M39" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="N39" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O39" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P39" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q39" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="R39" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>22</v>
       </c>
       <c r="B40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C40">
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="D40">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="E40">
         <v>10</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F40" t="s">
         <v>92</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>93</v>
       </c>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2">
-        <v>0</v>
-      </c>
+      <c r="H40" s="2">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="I40" s="2">
+        <v>0.54600000000000004</v>
+      </c>
+      <c r="J40" s="2"/>
       <c r="K40" s="2">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>2.3199999999999998</v>
       </c>
       <c r="L40" s="2">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>4.6399999999999997</v>
       </c>
       <c r="M40" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N40" t="s">
+        <v>0</v>
+      </c>
+      <c r="N40" s="2">
+        <f t="shared" si="4"/>
+        <v>11.6</v>
+      </c>
+      <c r="O40" s="2">
+        <f t="shared" si="5"/>
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="P40" s="2">
+        <f t="shared" si="6"/>
+        <v>4.6399999999999997</v>
+      </c>
+      <c r="Q40" s="2">
+        <f t="shared" si="7"/>
+        <v>6.9599999999999991</v>
+      </c>
+      <c r="R40" s="2">
+        <f t="shared" si="8"/>
+        <v>5.4600000000000009</v>
+      </c>
+      <c r="S40" t="s">
         <v>94</v>
       </c>
-      <c r="O40" t="s">
+      <c r="T40" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>23</v>
       </c>
       <c r="B41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C41">
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="D41">
-        <v>0</v>
-      </c>
-      <c r="E41" t="s">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41" t="s">
         <v>96</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>97</v>
       </c>
-      <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
-      <c r="J41" s="2">
-        <v>0</v>
-      </c>
+      <c r="J41" s="2"/>
       <c r="K41" s="2">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L41" s="2">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M41" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="N41" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O41" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P41" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q41" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="R41" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>24</v>
       </c>
@@ -2540,47 +3228,70 @@
         <v>2</v>
       </c>
       <c r="C42">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="D42">
+      <c r="E42">
         <v>10</v>
       </c>
-      <c r="E42" t="s">
+      <c r="F42" t="s">
         <v>98</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>99</v>
       </c>
-      <c r="G42" s="2">
+      <c r="H42" s="2">
         <v>1.05</v>
       </c>
-      <c r="H42" s="2">
+      <c r="I42" s="2">
         <v>0.41</v>
       </c>
-      <c r="I42" s="2">
+      <c r="J42" s="2">
         <v>0.26040000000000002</v>
       </c>
-      <c r="J42" s="2">
+      <c r="K42" s="2">
+        <f t="shared" si="2"/>
         <v>2.1</v>
       </c>
-      <c r="K42" s="2">
+      <c r="L42" s="2">
+        <f t="shared" si="3"/>
+        <v>4.2</v>
+      </c>
+      <c r="M42" s="2">
         <v>6.3</v>
       </c>
-      <c r="L42" s="2">
+      <c r="N42" s="2">
+        <f t="shared" si="4"/>
         <v>10.5</v>
       </c>
-      <c r="M42" s="2">
-        <f t="shared" si="0"/>
+      <c r="O42" s="2">
+        <f t="shared" si="5"/>
+        <v>2.1</v>
+      </c>
+      <c r="P42" s="2">
+        <f t="shared" si="6"/>
+        <v>4.2</v>
+      </c>
+      <c r="Q42" s="2">
+        <f t="shared" si="7"/>
+        <v>6.3000000000000007</v>
+      </c>
+      <c r="R42" s="2">
+        <f t="shared" si="8"/>
         <v>4.0999999999999996</v>
       </c>
-      <c r="N42" t="s">
+      <c r="S42" t="s">
         <v>100</v>
       </c>
-      <c r="O42" t="s">
+      <c r="T42" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>25</v>
       </c>
@@ -2588,82 +3299,128 @@
         <v>1</v>
       </c>
       <c r="C43">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="D43">
+      <c r="E43">
         <v>4</v>
       </c>
-      <c r="E43" t="s">
+      <c r="F43" t="s">
         <v>102</v>
       </c>
-      <c r="F43" t="s">
+      <c r="G43" t="s">
         <v>103</v>
       </c>
-      <c r="G43" s="2">
+      <c r="H43" s="2">
         <v>2.1</v>
       </c>
-      <c r="H43" s="2"/>
       <c r="I43" s="2"/>
-      <c r="J43" s="2">
+      <c r="J43" s="2"/>
+      <c r="K43" s="2">
+        <f t="shared" si="2"/>
         <v>2.1</v>
       </c>
-      <c r="K43" s="2">
+      <c r="L43" s="2">
+        <f t="shared" si="3"/>
+        <v>4.2</v>
+      </c>
+      <c r="M43" s="2">
         <v>6.3</v>
       </c>
-      <c r="L43" s="2">
+      <c r="N43" s="2">
+        <f t="shared" si="4"/>
         <v>8.4</v>
       </c>
-      <c r="M43" s="2">
-        <f t="shared" si="0"/>
+      <c r="O43" s="2">
+        <f t="shared" si="5"/>
+        <v>2.1</v>
+      </c>
+      <c r="P43" s="2">
+        <f t="shared" si="6"/>
+        <v>4.2</v>
+      </c>
+      <c r="Q43" s="2">
+        <f t="shared" si="7"/>
+        <v>6.3000000000000007</v>
+      </c>
+      <c r="R43" s="2">
+        <f t="shared" si="8"/>
         <v>8.4</v>
       </c>
-      <c r="N43" t="s">
+      <c r="S43" t="s">
         <v>103</v>
       </c>
-      <c r="O43" t="s">
+      <c r="T43" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>26</v>
       </c>
       <c r="B44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C44">
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="D44">
-        <v>0</v>
-      </c>
-      <c r="E44" t="s">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44" t="s">
         <v>105</v>
       </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>106</v>
       </c>
-      <c r="G44" s="2"/>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
-      <c r="J44" s="2">
-        <v>0</v>
-      </c>
+      <c r="J44" s="2"/>
       <c r="K44" s="2">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L44" s="2">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M44" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N44" t="s">
+        <v>0</v>
+      </c>
+      <c r="N44" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O44" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P44" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q44" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="R44" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="S44" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>27</v>
       </c>
@@ -2671,43 +3428,66 @@
         <v>1</v>
       </c>
       <c r="C45">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="D45">
+      <c r="E45">
         <v>4</v>
       </c>
-      <c r="E45" t="s">
+      <c r="F45" t="s">
         <v>107</v>
       </c>
-      <c r="F45" t="s">
+      <c r="G45" t="s">
         <v>108</v>
       </c>
-      <c r="G45" s="2">
+      <c r="H45" s="2">
         <v>2.84</v>
       </c>
-      <c r="H45" s="2"/>
       <c r="I45" s="2"/>
-      <c r="J45" s="2">
+      <c r="J45" s="2"/>
+      <c r="K45" s="2">
+        <f t="shared" si="2"/>
         <v>2.84</v>
       </c>
-      <c r="K45" s="2">
+      <c r="L45" s="2">
+        <f t="shared" si="3"/>
+        <v>5.68</v>
+      </c>
+      <c r="M45" s="2">
         <v>8.52</v>
       </c>
-      <c r="L45" s="2">
+      <c r="N45" s="2">
+        <f t="shared" si="4"/>
         <v>11.36</v>
       </c>
-      <c r="M45" s="2">
-        <f t="shared" si="0"/>
+      <c r="O45" s="2">
+        <f t="shared" si="5"/>
+        <v>2.84</v>
+      </c>
+      <c r="P45" s="2">
+        <f t="shared" si="6"/>
+        <v>5.68</v>
+      </c>
+      <c r="Q45" s="2">
+        <f t="shared" si="7"/>
+        <v>8.52</v>
+      </c>
+      <c r="R45" s="2">
+        <f t="shared" si="8"/>
         <v>11.36</v>
       </c>
-      <c r="N45" t="s">
+      <c r="S45" t="s">
         <v>108</v>
       </c>
-      <c r="O45" t="s">
+      <c r="T45" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>28</v>
       </c>
@@ -2715,43 +3495,66 @@
         <v>1</v>
       </c>
       <c r="C46">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="D46">
+      <c r="E46">
         <v>4</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F46" t="s">
         <v>110</v>
       </c>
-      <c r="F46" t="s">
+      <c r="G46" t="s">
         <v>111</v>
       </c>
-      <c r="G46" s="2">
+      <c r="H46" s="2">
         <v>3.78</v>
       </c>
-      <c r="H46" s="2"/>
       <c r="I46" s="2"/>
-      <c r="J46" s="2">
+      <c r="J46" s="2"/>
+      <c r="K46" s="2">
+        <f t="shared" si="2"/>
         <v>3.78</v>
       </c>
-      <c r="K46" s="2">
+      <c r="L46" s="2">
+        <f t="shared" si="3"/>
+        <v>7.56</v>
+      </c>
+      <c r="M46" s="2">
         <v>11.34</v>
       </c>
-      <c r="L46" s="2">
+      <c r="N46" s="2">
+        <f t="shared" si="4"/>
         <v>15.12</v>
       </c>
-      <c r="M46" s="2">
-        <f t="shared" si="0"/>
+      <c r="O46" s="2">
+        <f t="shared" si="5"/>
+        <v>3.78</v>
+      </c>
+      <c r="P46" s="2">
+        <f t="shared" si="6"/>
+        <v>7.56</v>
+      </c>
+      <c r="Q46" s="2">
+        <f t="shared" si="7"/>
+        <v>11.34</v>
+      </c>
+      <c r="R46" s="2">
+        <f t="shared" si="8"/>
         <v>15.12</v>
       </c>
-      <c r="N46" t="s">
+      <c r="S46" t="s">
         <v>111</v>
       </c>
-      <c r="O46" t="s">
+      <c r="T46" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>29</v>
       </c>
@@ -2759,45 +3562,68 @@
         <v>2</v>
       </c>
       <c r="C47">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="D47">
+      <c r="E47">
         <v>10</v>
       </c>
-      <c r="E47" t="s">
+      <c r="F47" t="s">
         <v>113</v>
       </c>
-      <c r="F47" t="s">
+      <c r="G47" t="s">
         <v>114</v>
       </c>
-      <c r="G47" s="2">
+      <c r="H47" s="2">
         <v>3.47</v>
       </c>
-      <c r="H47" s="2">
+      <c r="I47" s="2">
         <v>2.3210000000000002</v>
       </c>
-      <c r="I47" s="2"/>
-      <c r="J47" s="2">
+      <c r="J47" s="2"/>
+      <c r="K47" s="2">
+        <f t="shared" si="2"/>
         <v>6.94</v>
       </c>
-      <c r="K47" s="2">
+      <c r="L47" s="2">
+        <f t="shared" si="3"/>
+        <v>13.88</v>
+      </c>
+      <c r="M47" s="2">
         <v>20.82</v>
       </c>
-      <c r="L47" s="2">
+      <c r="N47" s="2">
+        <f t="shared" si="4"/>
         <v>34.700000000000003</v>
       </c>
-      <c r="M47" s="2">
-        <f t="shared" si="0"/>
+      <c r="O47" s="2">
+        <f t="shared" si="5"/>
+        <v>6.94</v>
+      </c>
+      <c r="P47" s="2">
+        <f t="shared" si="6"/>
+        <v>13.88</v>
+      </c>
+      <c r="Q47" s="2">
+        <f t="shared" si="7"/>
+        <v>20.82</v>
+      </c>
+      <c r="R47" s="2">
+        <f t="shared" si="8"/>
         <v>23.21</v>
       </c>
-      <c r="N47" t="s">
+      <c r="S47" t="s">
         <v>115</v>
       </c>
-      <c r="O47" t="s">
+      <c r="T47" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>30</v>
       </c>
@@ -2805,72 +3631,136 @@
         <v>1</v>
       </c>
       <c r="C48">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="D48">
+      <c r="E48">
         <v>4</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="G48" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="G48" s="2">
+      <c r="H48" s="2">
         <v>12.6</v>
       </c>
-      <c r="H48" s="2"/>
       <c r="I48" s="2"/>
-      <c r="J48" s="2">
-        <f>G48*B48</f>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2">
+        <f t="shared" si="2"/>
         <v>12.6</v>
       </c>
-      <c r="K48" s="2">
-        <f>G48*C48</f>
+      <c r="L48" s="2">
+        <f t="shared" si="3"/>
+        <v>25.2</v>
+      </c>
+      <c r="M48" s="2">
+        <f>H48*D48</f>
         <v>37.799999999999997</v>
       </c>
-      <c r="L48" s="2">
-        <f>G48*D48</f>
+      <c r="N48" s="2">
+        <f t="shared" si="4"/>
         <v>50.4</v>
       </c>
-      <c r="M48" s="2">
-        <f t="shared" si="0"/>
+      <c r="O48" s="2">
+        <f t="shared" si="5"/>
+        <v>12.6</v>
+      </c>
+      <c r="P48" s="2">
+        <f t="shared" si="6"/>
+        <v>25.2</v>
+      </c>
+      <c r="Q48" s="2">
+        <f t="shared" si="7"/>
+        <v>37.799999999999997</v>
+      </c>
+      <c r="R48" s="2">
+        <f t="shared" si="8"/>
         <v>50.4</v>
       </c>
-      <c r="N48" s="1" t="s">
+      <c r="S48" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="O48" t="s">
+      <c r="T48" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B49">
-        <v>69</v>
+        <f>SUM(B15:B48)</f>
+        <v>71</v>
       </c>
       <c r="C49">
-        <v>207</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="H49" s="2"/>
+        <f>SUM(C15:C48)</f>
+        <v>142</v>
+      </c>
+      <c r="D49">
+        <f>SUM(D15:D48)</f>
+        <v>213</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>140</v>
+      </c>
       <c r="I49" s="2"/>
-      <c r="J49" s="2">
-        <f>SUM(J15:J48)</f>
-        <v>222.51999999999995</v>
-      </c>
+      <c r="J49" s="2"/>
       <c r="K49" s="2">
         <f>SUM(K15:K48)</f>
+        <v>230.1</v>
+      </c>
+      <c r="L49" s="2">
+        <f>SUM(L15:L48)</f>
+        <v>460.2</v>
+      </c>
+      <c r="M49" s="2">
+        <f>SUM(M15:M48)</f>
         <v>667.55999999999983</v>
       </c>
-      <c r="L49" s="3">
-        <f>SUM(L15:L48)</f>
-        <v>939.61</v>
-      </c>
-      <c r="M49" s="3">
-        <f>SUM(M15:M48)</f>
-        <v>795.81999999999994</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="N49" s="2">
+        <f t="shared" ref="N49:Q49" si="9">SUM(N15:N48)</f>
+        <v>951.21</v>
+      </c>
+      <c r="O49" s="2">
+        <f t="shared" si="9"/>
+        <v>221.40299999999999</v>
+      </c>
+      <c r="P49" s="2">
+        <f t="shared" si="9"/>
+        <v>427.44600000000003</v>
+      </c>
+      <c r="Q49" s="2">
+        <f t="shared" si="9"/>
+        <v>641.16899999999998</v>
+      </c>
+      <c r="R49" s="5">
+        <f>SUM(R15:R48)</f>
+        <v>801.28</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="H50" t="s">
+        <v>117</v>
+      </c>
+      <c r="O50" s="2">
+        <f>O49+IF(O49&gt;=420,0,145)</f>
+        <v>366.40300000000002</v>
+      </c>
+      <c r="P50" s="2">
+        <f t="shared" ref="P50:R50" si="10">P49+IF(P49&gt;=420,0,145)</f>
+        <v>427.44600000000003</v>
+      </c>
+      <c r="Q50" s="2">
+        <f t="shared" si="10"/>
+        <v>641.16899999999998</v>
+      </c>
+      <c r="R50" s="3">
+        <f t="shared" si="10"/>
+        <v>801.28</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B51" s="4" t="s">
         <v>118</v>
       </c>
@@ -2887,132 +3777,168 @@
       <c r="M51" s="4"/>
       <c r="N51" s="4"/>
       <c r="O51" s="4"/>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P51" s="4"/>
+      <c r="Q51" s="4"/>
+      <c r="R51" s="4"/>
+      <c r="S51" s="4"/>
+      <c r="T51" s="4"/>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>31</v>
       </c>
       <c r="B52">
         <v>1</v>
       </c>
-      <c r="C52">
-        <v>2</v>
-      </c>
       <c r="D52">
         <v>2</v>
       </c>
-      <c r="F52" t="s">
+      <c r="E52">
+        <v>2</v>
+      </c>
+      <c r="G52" t="s">
         <v>119</v>
       </c>
-      <c r="G52" s="2">
+      <c r="H52" s="2">
         <v>5.99</v>
       </c>
-      <c r="H52" s="2"/>
       <c r="I52" s="2"/>
-      <c r="J52" s="2">
-        <f>G52*B52</f>
+      <c r="J52" s="2"/>
+      <c r="L52" s="2"/>
+      <c r="N52" s="2">
+        <f>H52*E52</f>
+        <v>11.98</v>
+      </c>
+      <c r="O52" s="2">
+        <f>H52*B52</f>
         <v>5.99</v>
       </c>
-      <c r="K52" s="2">
-        <f>G52*C52</f>
+      <c r="P52" s="2">
+        <f>H52*D52</f>
         <v>11.98</v>
       </c>
-      <c r="L52" s="2">
-        <f>G52*D52</f>
+      <c r="Q52" s="2"/>
+      <c r="R52" s="2">
+        <f>H52*E52</f>
         <v>11.98</v>
       </c>
-      <c r="M52" s="2"/>
-      <c r="O52" t="s">
+      <c r="T52" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>32</v>
       </c>
       <c r="B53">
         <v>1</v>
       </c>
-      <c r="C53">
-        <v>2</v>
-      </c>
       <c r="D53">
         <v>2</v>
       </c>
-      <c r="F53" t="s">
+      <c r="E53">
+        <v>2</v>
+      </c>
+      <c r="G53" t="s">
         <v>121</v>
       </c>
-      <c r="G53" s="2">
+      <c r="H53" s="2">
         <v>7.98</v>
       </c>
-      <c r="H53" s="2"/>
       <c r="I53" s="2"/>
-      <c r="J53" s="2">
-        <f>G53*B53</f>
+      <c r="J53" s="2"/>
+      <c r="L53" s="2"/>
+      <c r="N53" s="2">
+        <f>H53*E53</f>
+        <v>15.96</v>
+      </c>
+      <c r="O53" s="2">
+        <f>H53*B53</f>
         <v>7.98</v>
       </c>
-      <c r="K53" s="2">
-        <f t="shared" ref="K53" si="1">G53*C53</f>
+      <c r="P53" s="2">
+        <f>H53*D53</f>
         <v>15.96</v>
       </c>
-      <c r="L53" s="2">
-        <f t="shared" ref="L53" si="2">G53*D53</f>
+      <c r="Q53" s="2"/>
+      <c r="R53" s="2">
+        <f>H53*E53</f>
         <v>15.96</v>
       </c>
-      <c r="M53" s="2"/>
-      <c r="O53" t="s">
+      <c r="T53" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>33</v>
       </c>
       <c r="B54">
         <v>1</v>
       </c>
-      <c r="C54">
-        <v>3</v>
-      </c>
       <c r="D54">
         <v>3</v>
       </c>
-      <c r="F54" t="s">
+      <c r="E54">
+        <v>3</v>
+      </c>
+      <c r="G54" t="s">
         <v>130</v>
       </c>
-      <c r="G54" s="2">
+      <c r="H54" s="2">
         <v>3.89</v>
       </c>
-      <c r="H54" s="2"/>
       <c r="I54" s="2"/>
-      <c r="J54" s="2">
-        <f>G54*B54</f>
+      <c r="J54" s="2"/>
+      <c r="L54" s="2"/>
+      <c r="N54" s="2">
+        <f>H54*E54</f>
+        <v>11.67</v>
+      </c>
+      <c r="O54" s="2">
+        <f>H54*B54</f>
         <v>3.89</v>
       </c>
-      <c r="K54" s="2">
-        <f t="shared" ref="K54" si="3">G54*C54</f>
+      <c r="P54" s="2">
+        <f>H54*D54</f>
         <v>11.67</v>
       </c>
-      <c r="L54" s="2">
-        <f t="shared" ref="L54" si="4">G54*D54</f>
+      <c r="Q54" s="2"/>
+      <c r="R54" s="2">
+        <f>H54*E54</f>
         <v>11.67</v>
       </c>
-      <c r="M54" s="2"/>
-      <c r="O54" t="s">
+      <c r="T54" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="L55" s="2">
-        <f>SUM(L52:L54)</f>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="N55" s="2">
+        <f>SUM(N52:N54)</f>
         <v>39.61</v>
       </c>
-      <c r="M55" s="2"/>
+      <c r="O55" s="2"/>
+      <c r="P55" s="2"/>
+      <c r="Q55" s="2"/>
+      <c r="R55" s="2">
+        <f>SUM(R52:R54)</f>
+        <v>39.61</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="Q57" t="s">
+        <v>142</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B51:O51"/>
+    <mergeCell ref="B51:T51"/>
   </mergeCells>
+  <conditionalFormatting sqref="C49 A15:T48">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$B15=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Final cost optimisation by cutting margins on expensive components
</commit_message>
<xml_diff>
--- a/PCB-Node1/BOM_BYGGERNNODE1.xlsx
+++ b/PCB-Node1/BOM_BYGGERNNODE1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benja\Documents\Byggeren\TTK4155_Ping_Pong_Project\PCB-Node1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1247A2B-7BA5-4F54-BA69-154ACCEE679B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D99AEB2-DE69-4CCD-9795-4610505DB422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2720" yWindow="440" windowWidth="20760" windowHeight="14220" xr2:uid="{17AFD791-CEED-4828-96C0-A0F19B8C3E72}"/>
   </bookViews>
@@ -443,9 +443,6 @@
     <t>2 Board cost</t>
   </si>
   <si>
-    <t>parts Total:</t>
-  </si>
-  <si>
     <t>1 Order Quantity</t>
   </si>
   <si>
@@ -471,6 +468,9 @@
   </si>
   <si>
     <t>3 Order cost</t>
+  </si>
+  <si>
+    <t>All parts:</t>
   </si>
 </sst>
 </file>
@@ -994,9 +994,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
@@ -1006,6 +1003,9 @@
     <xf numFmtId="164" fontId="16" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="16" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1051,7 +1051,13 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="2" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1391,11 +1397,11 @@
   <dimension ref="A1:X55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="K37" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="H47" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A10" sqref="A10"/>
       <selection pane="topRight" activeCell="B10" sqref="B10"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="T58" sqref="T58"/>
+      <selection pane="bottomRight" activeCell="K61" sqref="K61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1448,13 +1454,13 @@
         <v>6</v>
       </c>
       <c r="E12" t="s">
+        <v>136</v>
+      </c>
+      <c r="F12" t="s">
         <v>137</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>138</v>
-      </c>
-      <c r="G12" t="s">
-        <v>139</v>
       </c>
       <c r="H12" t="s">
         <v>7</v>
@@ -1484,22 +1490,22 @@
         <v>12</v>
       </c>
       <c r="Q12" t="s">
+        <v>139</v>
+      </c>
+      <c r="R12" t="s">
         <v>140</v>
       </c>
-      <c r="R12" t="s">
+      <c r="S12" t="s">
         <v>141</v>
       </c>
-      <c r="S12" t="s">
+      <c r="T12" t="s">
         <v>142</v>
       </c>
-      <c r="T12" t="s">
+      <c r="U12" t="s">
         <v>143</v>
       </c>
-      <c r="U12" t="s">
+      <c r="V12" t="s">
         <v>144</v>
-      </c>
-      <c r="V12" t="s">
-        <v>145</v>
       </c>
       <c r="W12" t="s">
         <v>13</v>
@@ -1517,24 +1523,24 @@
       <c r="A15">
         <v>1</v>
       </c>
-      <c r="B15" s="6">
-        <v>2</v>
-      </c>
-      <c r="C15" s="4">
+      <c r="B15" s="5">
+        <v>2</v>
+      </c>
+      <c r="C15" s="3">
         <f>B15*2</f>
         <v>4</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <f>B15*3</f>
         <v>6</v>
       </c>
-      <c r="E15" s="6">
-        <v>2</v>
-      </c>
-      <c r="F15" s="4">
+      <c r="E15" s="5">
+        <v>2</v>
+      </c>
+      <c r="F15" s="3">
         <v>4</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="4">
         <v>6</v>
       </c>
       <c r="H15" t="s">
@@ -1563,27 +1569,27 @@
         <f>G15*J15</f>
         <v>76.86</v>
       </c>
-      <c r="Q15" s="7">
+      <c r="Q15" s="6">
         <f>IF(B15&gt;=50,B15*L15,IF(B15&gt;=10,B15*K15,B15*J15))</f>
         <v>25.62</v>
       </c>
-      <c r="R15" s="9">
+      <c r="R15" s="8">
         <f>IF(C15&gt;=50,C15*L15,IF(C15&gt;=10,C15*K15,C15*J15))</f>
         <v>51.24</v>
       </c>
-      <c r="S15" s="11">
+      <c r="S15" s="10">
         <f>IF(D15&gt;=50,D15*L15,IF(D15&gt;=10,D15*K15,D15*J15))</f>
         <v>76.86</v>
       </c>
-      <c r="T15" s="7">
+      <c r="T15" s="6">
         <f>IF(E15&gt;=50,E15*L15,IF(E15&gt;=10,E15*K15,E15*J15))</f>
         <v>25.62</v>
       </c>
-      <c r="U15" s="9">
+      <c r="U15" s="8">
         <f>IF(F15&gt;=50,F15*L15,IF(F15&gt;=10,F15*K15,F15*J15))</f>
         <v>51.24</v>
       </c>
-      <c r="V15" s="11">
+      <c r="V15" s="10">
         <f>IF(G15&gt;=50,G15*L15,IF(G15&gt;=10,G15*K15,G15*J15))</f>
         <v>76.86</v>
       </c>
@@ -1598,26 +1604,26 @@
       <c r="A16">
         <v>2</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="5">
         <v>1</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="3">
         <f t="shared" ref="C16:C48" si="0">B16*2</f>
         <v>2</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="4">
         <f t="shared" ref="D16:D48" si="1">B16*3</f>
         <v>3</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="5">
         <f>IF(B16&gt;0,B16+1,0)</f>
         <v>2</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="3">
         <f>IF(C16&gt;0,C16+1,0)</f>
         <v>3</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16" s="4">
         <f>IF(D16&gt;0,D16+1,0)</f>
         <v>4</v>
       </c>
@@ -1647,27 +1653,27 @@
         <f t="shared" ref="P16:P48" si="4">G16*J16</f>
         <v>40.76</v>
       </c>
-      <c r="Q16" s="7">
+      <c r="Q16" s="6">
         <f t="shared" ref="Q16:Q48" si="5">IF(B16&gt;=50,B16*L16,IF(B16&gt;=10,B16*K16,B16*J16))</f>
         <v>10.19</v>
       </c>
-      <c r="R16" s="9">
+      <c r="R16" s="8">
         <f t="shared" ref="R16:R48" si="6">IF(C16&gt;=50,C16*L16,IF(C16&gt;=10,C16*K16,C16*J16))</f>
         <v>20.38</v>
       </c>
-      <c r="S16" s="11">
+      <c r="S16" s="10">
         <f t="shared" ref="S16:S48" si="7">IF(D16&gt;=50,D16*L16,IF(D16&gt;=10,D16*K16,D16*J16))</f>
         <v>30.57</v>
       </c>
-      <c r="T16" s="7">
+      <c r="T16" s="6">
         <f t="shared" ref="T16:T48" si="8">IF(E16&gt;=50,E16*L16,IF(E16&gt;=10,E16*K16,E16*J16))</f>
         <v>20.38</v>
       </c>
-      <c r="U16" s="9">
+      <c r="U16" s="8">
         <f t="shared" ref="U16:U48" si="9">IF(F16&gt;=50,F16*L16,IF(F16&gt;=10,F16*K16,F16*J16))</f>
         <v>30.57</v>
       </c>
-      <c r="V16" s="11">
+      <c r="V16" s="10">
         <f t="shared" ref="V16:V48" si="10">IF(G16&gt;=50,G16*L16,IF(G16&gt;=10,G16*K16,G16*J16))</f>
         <v>40.76</v>
       </c>
@@ -1682,26 +1688,26 @@
       <c r="A17">
         <v>3</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="5">
         <v>1</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="4">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="5">
         <f t="shared" ref="E17:E48" si="11">IF(B17&gt;0,B17+1,0)</f>
         <v>2</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="3">
         <f t="shared" ref="F17:F48" si="12">IF(C17&gt;0,C17+1,0)</f>
         <v>3</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G17" s="4">
         <f t="shared" ref="G17:G48" si="13">IF(D17&gt;0,D17+1,0)</f>
         <v>4</v>
       </c>
@@ -1731,27 +1737,27 @@
         <f t="shared" si="4"/>
         <v>23.96</v>
       </c>
-      <c r="Q17" s="7">
+      <c r="Q17" s="6">
         <f t="shared" si="5"/>
         <v>5.99</v>
       </c>
-      <c r="R17" s="9">
+      <c r="R17" s="8">
         <f t="shared" si="6"/>
         <v>11.98</v>
       </c>
-      <c r="S17" s="11">
+      <c r="S17" s="10">
         <f t="shared" si="7"/>
         <v>17.97</v>
       </c>
-      <c r="T17" s="7">
+      <c r="T17" s="6">
         <f t="shared" si="8"/>
         <v>11.98</v>
       </c>
-      <c r="U17" s="9">
+      <c r="U17" s="8">
         <f t="shared" si="9"/>
         <v>17.97</v>
       </c>
-      <c r="V17" s="11">
+      <c r="V17" s="10">
         <f t="shared" si="10"/>
         <v>23.96</v>
       </c>
@@ -1766,26 +1772,26 @@
       <c r="A18">
         <v>4</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="5">
         <v>17</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="3">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="4">
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="5">
         <f t="shared" si="11"/>
         <v>18</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="3">
         <f t="shared" si="12"/>
         <v>35</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G18" s="4">
         <f t="shared" si="13"/>
         <v>52</v>
       </c>
@@ -1819,27 +1825,27 @@
         <f t="shared" si="4"/>
         <v>104</v>
       </c>
-      <c r="Q18" s="7">
+      <c r="Q18" s="6">
         <f t="shared" si="5"/>
         <v>31.603000000000002</v>
       </c>
-      <c r="R18" s="9">
+      <c r="R18" s="8">
         <f t="shared" si="6"/>
         <v>63.206000000000003</v>
       </c>
-      <c r="S18" s="11">
+      <c r="S18" s="10">
         <f t="shared" si="7"/>
         <v>94.808999999999997</v>
       </c>
-      <c r="T18" s="7">
+      <c r="T18" s="6">
         <f t="shared" si="8"/>
         <v>33.462000000000003</v>
       </c>
-      <c r="U18" s="9">
+      <c r="U18" s="8">
         <f t="shared" si="9"/>
         <v>65.064999999999998</v>
       </c>
-      <c r="V18" s="11">
+      <c r="V18" s="10">
         <f t="shared" si="10"/>
         <v>96.668000000000006</v>
       </c>
@@ -1851,24 +1857,24 @@
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="B19" s="6"/>
-      <c r="C19" s="4">
+      <c r="B19" s="5"/>
+      <c r="C19" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="5">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19" s="3">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="G19" s="5">
+      <c r="G19" s="4">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -1893,50 +1899,50 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Q19" s="7">
+      <c r="Q19" s="6">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R19" s="9">
+      <c r="R19" s="8">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="S19" s="11">
+      <c r="S19" s="10">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="T19" s="7">
+      <c r="T19" s="6">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="U19" s="9">
+      <c r="U19" s="8">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="V19" s="11">
+      <c r="V19" s="10">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="B20" s="6"/>
-      <c r="C20" s="4">
+      <c r="B20" s="5"/>
+      <c r="C20" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="5">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="3">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G20" s="4">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -1961,27 +1967,27 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Q20" s="7">
+      <c r="Q20" s="6">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R20" s="9">
+      <c r="R20" s="8">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="S20" s="11">
+      <c r="S20" s="10">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="T20" s="7">
+      <c r="T20" s="6">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="U20" s="9">
+      <c r="U20" s="8">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="V20" s="11">
+      <c r="V20" s="10">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -1990,26 +1996,26 @@
       <c r="A21">
         <v>5</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="5">
         <v>12</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="3">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="4">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="5">
         <f t="shared" si="11"/>
         <v>13</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21" s="3">
         <f t="shared" si="12"/>
         <v>25</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G21" s="4">
         <f t="shared" si="13"/>
         <v>37</v>
       </c>
@@ -2043,27 +2049,27 @@
         <f t="shared" si="4"/>
         <v>46.62</v>
       </c>
-      <c r="Q21" s="7">
+      <c r="Q21" s="6">
         <f t="shared" si="5"/>
         <v>8.82</v>
       </c>
-      <c r="R21" s="9">
+      <c r="R21" s="8">
         <f t="shared" si="6"/>
         <v>17.64</v>
       </c>
-      <c r="S21" s="11">
+      <c r="S21" s="10">
         <f t="shared" si="7"/>
         <v>26.46</v>
       </c>
-      <c r="T21" s="7">
+      <c r="T21" s="6">
         <f t="shared" si="8"/>
         <v>9.5549999999999997</v>
       </c>
-      <c r="U21" s="9">
+      <c r="U21" s="8">
         <f t="shared" si="9"/>
         <v>18.375</v>
       </c>
-      <c r="V21" s="11">
+      <c r="V21" s="10">
         <f t="shared" si="10"/>
         <v>27.195</v>
       </c>
@@ -2075,24 +2081,24 @@
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="B22" s="6"/>
-      <c r="C22" s="4">
+      <c r="B22" s="5"/>
+      <c r="C22" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="5">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22" s="3">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="G22" s="5">
+      <c r="G22" s="4">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -2117,27 +2123,27 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Q22" s="7">
+      <c r="Q22" s="6">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R22" s="9">
+      <c r="R22" s="8">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="S22" s="11">
+      <c r="S22" s="10">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="T22" s="7">
+      <c r="T22" s="6">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="U22" s="9">
+      <c r="U22" s="8">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="V22" s="11">
+      <c r="V22" s="10">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -2146,26 +2152,26 @@
       <c r="A23">
         <v>6</v>
       </c>
-      <c r="B23" s="6">
-        <v>2</v>
-      </c>
-      <c r="C23" s="4">
+      <c r="B23" s="5">
+        <v>2</v>
+      </c>
+      <c r="C23" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="4">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="5">
         <f t="shared" si="11"/>
         <v>3</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F23" s="3">
         <f t="shared" si="12"/>
         <v>5</v>
       </c>
-      <c r="G23" s="5">
+      <c r="G23" s="4">
         <f t="shared" si="13"/>
         <v>7</v>
       </c>
@@ -2199,27 +2205,27 @@
         <f t="shared" si="4"/>
         <v>7.3500000000000005</v>
       </c>
-      <c r="Q23" s="7">
+      <c r="Q23" s="6">
         <f t="shared" si="5"/>
         <v>2.1</v>
       </c>
-      <c r="R23" s="9">
+      <c r="R23" s="8">
         <f t="shared" si="6"/>
         <v>4.2</v>
       </c>
-      <c r="S23" s="11">
+      <c r="S23" s="10">
         <f t="shared" si="7"/>
         <v>6.3000000000000007</v>
       </c>
-      <c r="T23" s="7">
+      <c r="T23" s="6">
         <f t="shared" si="8"/>
         <v>3.1500000000000004</v>
       </c>
-      <c r="U23" s="9">
+      <c r="U23" s="8">
         <f t="shared" si="9"/>
         <v>5.25</v>
       </c>
-      <c r="V23" s="11">
+      <c r="V23" s="10">
         <f t="shared" si="10"/>
         <v>7.3500000000000005</v>
       </c>
@@ -2234,24 +2240,24 @@
       <c r="A24">
         <v>7</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="5">
         <v>1</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="3">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="4">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="5">
         <v>1</v>
       </c>
-      <c r="F24" s="4">
-        <v>2</v>
-      </c>
-      <c r="G24" s="5">
+      <c r="F24" s="3">
+        <v>2</v>
+      </c>
+      <c r="G24" s="4">
         <v>3</v>
       </c>
       <c r="H24" t="s">
@@ -2280,27 +2286,27 @@
         <f t="shared" si="4"/>
         <v>34.650000000000006</v>
       </c>
-      <c r="Q24" s="7">
+      <c r="Q24" s="6">
         <f t="shared" si="5"/>
         <v>11.55</v>
       </c>
-      <c r="R24" s="9">
+      <c r="R24" s="8">
         <f t="shared" si="6"/>
         <v>23.1</v>
       </c>
-      <c r="S24" s="11">
+      <c r="S24" s="10">
         <f t="shared" si="7"/>
         <v>34.650000000000006</v>
       </c>
-      <c r="T24" s="7">
+      <c r="T24" s="6">
         <f t="shared" si="8"/>
         <v>11.55</v>
       </c>
-      <c r="U24" s="9">
+      <c r="U24" s="8">
         <f t="shared" si="9"/>
         <v>23.1</v>
       </c>
-      <c r="V24" s="11">
+      <c r="V24" s="10">
         <f t="shared" si="10"/>
         <v>34.650000000000006</v>
       </c>
@@ -2315,24 +2321,24 @@
       <c r="A25">
         <v>8</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="5">
         <v>1</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="3">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="4">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="5">
         <v>1</v>
       </c>
-      <c r="F25" s="4">
-        <v>2</v>
-      </c>
-      <c r="G25" s="5">
+      <c r="F25" s="3">
+        <v>2</v>
+      </c>
+      <c r="G25" s="4">
         <v>3</v>
       </c>
       <c r="H25" t="s">
@@ -2361,27 +2367,27 @@
         <f t="shared" si="4"/>
         <v>12.299999999999999</v>
       </c>
-      <c r="Q25" s="7">
+      <c r="Q25" s="6">
         <f t="shared" si="5"/>
         <v>4.0999999999999996</v>
       </c>
-      <c r="R25" s="9">
+      <c r="R25" s="8">
         <f t="shared" si="6"/>
         <v>8.1999999999999993</v>
       </c>
-      <c r="S25" s="11">
+      <c r="S25" s="10">
         <f t="shared" si="7"/>
         <v>12.299999999999999</v>
       </c>
-      <c r="T25" s="7">
+      <c r="T25" s="6">
         <f t="shared" si="8"/>
         <v>4.0999999999999996</v>
       </c>
-      <c r="U25" s="9">
+      <c r="U25" s="8">
         <f t="shared" si="9"/>
         <v>8.1999999999999993</v>
       </c>
-      <c r="V25" s="11">
+      <c r="V25" s="10">
         <f t="shared" si="10"/>
         <v>12.299999999999999</v>
       </c>
@@ -2396,24 +2402,24 @@
       <c r="A26">
         <v>9</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="5">
         <v>1</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26" s="3">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="4">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="5">
         <v>1</v>
       </c>
-      <c r="F26" s="4">
-        <v>2</v>
-      </c>
-      <c r="G26" s="5">
+      <c r="F26" s="3">
+        <v>2</v>
+      </c>
+      <c r="G26" s="4">
         <v>3</v>
       </c>
       <c r="H26" t="s">
@@ -2442,27 +2448,27 @@
         <f t="shared" si="4"/>
         <v>17.34</v>
       </c>
-      <c r="Q26" s="7">
+      <c r="Q26" s="6">
         <f t="shared" si="5"/>
         <v>5.78</v>
       </c>
-      <c r="R26" s="9">
+      <c r="R26" s="8">
         <f t="shared" si="6"/>
         <v>11.56</v>
       </c>
-      <c r="S26" s="11">
+      <c r="S26" s="10">
         <f t="shared" si="7"/>
         <v>17.34</v>
       </c>
-      <c r="T26" s="7">
+      <c r="T26" s="6">
         <f t="shared" si="8"/>
         <v>5.78</v>
       </c>
-      <c r="U26" s="9">
+      <c r="U26" s="8">
         <f t="shared" si="9"/>
         <v>11.56</v>
       </c>
-      <c r="V26" s="11">
+      <c r="V26" s="10">
         <f t="shared" si="10"/>
         <v>17.34</v>
       </c>
@@ -2477,24 +2483,24 @@
       <c r="A27">
         <v>10</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="5">
         <v>1</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C27" s="3">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D27" s="5">
+      <c r="D27" s="4">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="5">
         <v>1</v>
       </c>
-      <c r="F27" s="4">
-        <v>2</v>
-      </c>
-      <c r="G27" s="5">
+      <c r="F27" s="3">
+        <v>2</v>
+      </c>
+      <c r="G27" s="4">
         <v>3</v>
       </c>
       <c r="H27" t="s">
@@ -2523,27 +2529,27 @@
         <f t="shared" si="4"/>
         <v>17.64</v>
       </c>
-      <c r="Q27" s="7">
+      <c r="Q27" s="6">
         <f t="shared" si="5"/>
         <v>5.88</v>
       </c>
-      <c r="R27" s="9">
+      <c r="R27" s="8">
         <f t="shared" si="6"/>
         <v>11.76</v>
       </c>
-      <c r="S27" s="11">
+      <c r="S27" s="10">
         <f t="shared" si="7"/>
         <v>17.64</v>
       </c>
-      <c r="T27" s="7">
+      <c r="T27" s="6">
         <f t="shared" si="8"/>
         <v>5.88</v>
       </c>
-      <c r="U27" s="9">
+      <c r="U27" s="8">
         <f t="shared" si="9"/>
         <v>11.76</v>
       </c>
-      <c r="V27" s="11">
+      <c r="V27" s="10">
         <f t="shared" si="10"/>
         <v>17.64</v>
       </c>
@@ -2558,24 +2564,24 @@
       <c r="A28">
         <v>11</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="5">
         <v>1</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="3">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D28" s="5">
+      <c r="D28" s="4">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="5">
         <v>1</v>
       </c>
-      <c r="F28" s="4">
-        <v>2</v>
-      </c>
-      <c r="G28" s="5">
+      <c r="F28" s="3">
+        <v>2</v>
+      </c>
+      <c r="G28" s="4">
         <v>3</v>
       </c>
       <c r="H28" t="s">
@@ -2604,27 +2610,27 @@
         <f t="shared" si="4"/>
         <v>16.71</v>
       </c>
-      <c r="Q28" s="7">
+      <c r="Q28" s="6">
         <f t="shared" si="5"/>
         <v>5.57</v>
       </c>
-      <c r="R28" s="9">
+      <c r="R28" s="8">
         <f t="shared" si="6"/>
         <v>11.14</v>
       </c>
-      <c r="S28" s="11">
+      <c r="S28" s="10">
         <f t="shared" si="7"/>
         <v>16.71</v>
       </c>
-      <c r="T28" s="7">
+      <c r="T28" s="6">
         <f t="shared" si="8"/>
         <v>5.57</v>
       </c>
-      <c r="U28" s="9">
+      <c r="U28" s="8">
         <f t="shared" si="9"/>
         <v>11.14</v>
       </c>
-      <c r="V28" s="11">
+      <c r="V28" s="10">
         <f t="shared" si="10"/>
         <v>16.71</v>
       </c>
@@ -2639,24 +2645,24 @@
       <c r="A29">
         <v>12</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="5">
         <v>1</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29" s="3">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D29" s="5">
+      <c r="D29" s="4">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="5">
         <v>1</v>
       </c>
-      <c r="F29" s="4">
-        <v>2</v>
-      </c>
-      <c r="G29" s="5">
+      <c r="F29" s="3">
+        <v>2</v>
+      </c>
+      <c r="G29" s="4">
         <v>3</v>
       </c>
       <c r="H29" t="s">
@@ -2685,27 +2691,27 @@
         <f t="shared" si="4"/>
         <v>11.97</v>
       </c>
-      <c r="Q29" s="7">
+      <c r="Q29" s="6">
         <f t="shared" si="5"/>
         <v>3.99</v>
       </c>
-      <c r="R29" s="9">
+      <c r="R29" s="8">
         <f t="shared" si="6"/>
         <v>7.98</v>
       </c>
-      <c r="S29" s="11">
+      <c r="S29" s="10">
         <f t="shared" si="7"/>
         <v>11.97</v>
       </c>
-      <c r="T29" s="7">
+      <c r="T29" s="6">
         <f t="shared" si="8"/>
         <v>3.99</v>
       </c>
-      <c r="U29" s="9">
+      <c r="U29" s="8">
         <f t="shared" si="9"/>
         <v>7.98</v>
       </c>
-      <c r="V29" s="11">
+      <c r="V29" s="10">
         <f t="shared" si="10"/>
         <v>11.97</v>
       </c>
@@ -2720,24 +2726,24 @@
       <c r="A30">
         <v>13</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B30" s="5">
         <v>1</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30" s="3">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D30" s="5">
+      <c r="D30" s="4">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E30" s="5">
         <v>1</v>
       </c>
-      <c r="F30" s="4">
-        <v>2</v>
-      </c>
-      <c r="G30" s="5">
+      <c r="F30" s="3">
+        <v>2</v>
+      </c>
+      <c r="G30" s="4">
         <v>3</v>
       </c>
       <c r="H30" t="s">
@@ -2766,27 +2772,27 @@
         <f t="shared" si="4"/>
         <v>9.7799999999999994</v>
       </c>
-      <c r="Q30" s="7">
+      <c r="Q30" s="6">
         <f t="shared" si="5"/>
         <v>3.26</v>
       </c>
-      <c r="R30" s="9">
+      <c r="R30" s="8">
         <f t="shared" si="6"/>
         <v>6.52</v>
       </c>
-      <c r="S30" s="11">
+      <c r="S30" s="10">
         <f t="shared" si="7"/>
         <v>9.7799999999999994</v>
       </c>
-      <c r="T30" s="7">
+      <c r="T30" s="6">
         <f t="shared" si="8"/>
         <v>3.26</v>
       </c>
-      <c r="U30" s="9">
+      <c r="U30" s="8">
         <f t="shared" si="9"/>
         <v>6.52</v>
       </c>
-      <c r="V30" s="11">
+      <c r="V30" s="10">
         <f t="shared" si="10"/>
         <v>9.7799999999999994</v>
       </c>
@@ -2801,24 +2807,24 @@
       <c r="A31">
         <v>14</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="5">
         <v>1</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C31" s="3">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D31" s="5">
+      <c r="D31" s="4">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="5">
         <v>1</v>
       </c>
-      <c r="F31" s="4">
-        <v>2</v>
-      </c>
-      <c r="G31" s="5">
+      <c r="F31" s="3">
+        <v>2</v>
+      </c>
+      <c r="G31" s="4">
         <v>3</v>
       </c>
       <c r="H31" t="s">
@@ -2847,27 +2853,27 @@
         <f t="shared" si="4"/>
         <v>37.17</v>
       </c>
-      <c r="Q31" s="7">
+      <c r="Q31" s="6">
         <f t="shared" si="5"/>
         <v>12.39</v>
       </c>
-      <c r="R31" s="9">
+      <c r="R31" s="8">
         <f t="shared" si="6"/>
         <v>24.78</v>
       </c>
-      <c r="S31" s="11">
+      <c r="S31" s="10">
         <f t="shared" si="7"/>
         <v>37.17</v>
       </c>
-      <c r="T31" s="7">
+      <c r="T31" s="6">
         <f t="shared" si="8"/>
         <v>12.39</v>
       </c>
-      <c r="U31" s="9">
+      <c r="U31" s="8">
         <f t="shared" si="9"/>
         <v>24.78</v>
       </c>
-      <c r="V31" s="11">
+      <c r="V31" s="10">
         <f t="shared" si="10"/>
         <v>37.17</v>
       </c>
@@ -2882,24 +2888,24 @@
       <c r="A32">
         <v>15</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B32" s="5">
         <v>1</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="3">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D32" s="5">
+      <c r="D32" s="4">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E32" s="5">
         <v>1</v>
       </c>
-      <c r="F32" s="4">
-        <v>2</v>
-      </c>
-      <c r="G32" s="5">
+      <c r="F32" s="3">
+        <v>2</v>
+      </c>
+      <c r="G32" s="4">
         <v>3</v>
       </c>
       <c r="H32" t="s">
@@ -2928,27 +2934,27 @@
         <f t="shared" si="4"/>
         <v>34.650000000000006</v>
       </c>
-      <c r="Q32" s="7">
+      <c r="Q32" s="6">
         <f t="shared" si="5"/>
         <v>11.55</v>
       </c>
-      <c r="R32" s="9">
+      <c r="R32" s="8">
         <f t="shared" si="6"/>
         <v>23.1</v>
       </c>
-      <c r="S32" s="11">
+      <c r="S32" s="10">
         <f t="shared" si="7"/>
         <v>34.650000000000006</v>
       </c>
-      <c r="T32" s="7">
+      <c r="T32" s="6">
         <f t="shared" si="8"/>
         <v>11.55</v>
       </c>
-      <c r="U32" s="9">
+      <c r="U32" s="8">
         <f t="shared" si="9"/>
         <v>23.1</v>
       </c>
-      <c r="V32" s="11">
+      <c r="V32" s="10">
         <f t="shared" si="10"/>
         <v>34.650000000000006</v>
       </c>
@@ -2963,26 +2969,24 @@
       <c r="A33">
         <v>16</v>
       </c>
-      <c r="B33" s="6">
+      <c r="B33" s="5">
         <v>1</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33" s="3">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D33" s="5">
+      <c r="D33" s="4">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="E33" s="6">
-        <f t="shared" si="11"/>
-        <v>2</v>
-      </c>
-      <c r="F33" s="4">
-        <f t="shared" si="12"/>
-        <v>3</v>
-      </c>
-      <c r="G33" s="5">
+      <c r="E33" s="5">
+        <v>1</v>
+      </c>
+      <c r="F33" s="3">
+        <v>2</v>
+      </c>
+      <c r="G33" s="4">
         <v>3</v>
       </c>
       <c r="H33" t="s">
@@ -3011,27 +3015,27 @@
         <f t="shared" si="4"/>
         <v>51.36</v>
       </c>
-      <c r="Q33" s="7">
+      <c r="Q33" s="6">
         <f t="shared" si="5"/>
         <v>17.12</v>
       </c>
-      <c r="R33" s="9">
+      <c r="R33" s="8">
         <f t="shared" si="6"/>
         <v>34.24</v>
       </c>
-      <c r="S33" s="11">
+      <c r="S33" s="10">
         <f t="shared" si="7"/>
         <v>51.36</v>
       </c>
-      <c r="T33" s="7">
+      <c r="T33" s="6">
         <f t="shared" si="8"/>
+        <v>17.12</v>
+      </c>
+      <c r="U33" s="8">
+        <f t="shared" si="9"/>
         <v>34.24</v>
       </c>
-      <c r="U33" s="9">
-        <f t="shared" si="9"/>
-        <v>51.36</v>
-      </c>
-      <c r="V33" s="11">
+      <c r="V33" s="10">
         <f t="shared" si="10"/>
         <v>51.36</v>
       </c>
@@ -3046,26 +3050,26 @@
       <c r="A34">
         <v>17</v>
       </c>
-      <c r="B34" s="6">
+      <c r="B34" s="5">
         <v>1</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C34" s="3">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D34" s="5">
+      <c r="D34" s="4">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="E34" s="6">
+      <c r="E34" s="5">
         <f t="shared" si="11"/>
         <v>2</v>
       </c>
-      <c r="F34" s="4">
+      <c r="F34" s="3">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="G34" s="5">
+      <c r="G34" s="4">
         <v>3</v>
       </c>
       <c r="H34" t="s">
@@ -3094,27 +3098,27 @@
         <f t="shared" si="4"/>
         <v>14.82</v>
       </c>
-      <c r="Q34" s="7">
+      <c r="Q34" s="6">
         <f t="shared" si="5"/>
         <v>4.9400000000000004</v>
       </c>
-      <c r="R34" s="9">
+      <c r="R34" s="8">
         <f t="shared" si="6"/>
         <v>9.8800000000000008</v>
       </c>
-      <c r="S34" s="11">
+      <c r="S34" s="10">
         <f t="shared" si="7"/>
         <v>14.82</v>
       </c>
-      <c r="T34" s="7">
+      <c r="T34" s="6">
         <f t="shared" si="8"/>
         <v>9.8800000000000008</v>
       </c>
-      <c r="U34" s="9">
+      <c r="U34" s="8">
         <f t="shared" si="9"/>
         <v>14.82</v>
       </c>
-      <c r="V34" s="11">
+      <c r="V34" s="10">
         <f t="shared" si="10"/>
         <v>14.82</v>
       </c>
@@ -3129,26 +3133,26 @@
       <c r="A35">
         <v>18</v>
       </c>
-      <c r="B35" s="6">
+      <c r="B35" s="5">
         <v>3</v>
       </c>
-      <c r="C35" s="4">
+      <c r="C35" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="D35" s="5">
+      <c r="D35" s="4">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E35" s="5">
         <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="F35" s="4">
+      <c r="F35" s="3">
         <f t="shared" si="12"/>
         <v>7</v>
       </c>
-      <c r="G35" s="5">
+      <c r="G35" s="4">
         <f t="shared" si="13"/>
         <v>10</v>
       </c>
@@ -3182,27 +3186,27 @@
         <f t="shared" si="4"/>
         <v>18.899999999999999</v>
       </c>
-      <c r="Q35" s="7">
+      <c r="Q35" s="6">
         <f t="shared" si="5"/>
         <v>5.67</v>
       </c>
-      <c r="R35" s="9">
+      <c r="R35" s="8">
         <f t="shared" si="6"/>
         <v>11.34</v>
       </c>
-      <c r="S35" s="11">
+      <c r="S35" s="10">
         <f t="shared" si="7"/>
         <v>17.009999999999998</v>
       </c>
-      <c r="T35" s="7">
+      <c r="T35" s="6">
         <f t="shared" si="8"/>
         <v>7.56</v>
       </c>
-      <c r="U35" s="9">
+      <c r="U35" s="8">
         <f t="shared" si="9"/>
         <v>13.229999999999999</v>
       </c>
-      <c r="V35" s="11">
+      <c r="V35" s="10">
         <f t="shared" si="10"/>
         <v>18.899999999999999</v>
       </c>
@@ -3217,26 +3221,26 @@
       <c r="A36">
         <v>19</v>
       </c>
-      <c r="B36" s="6">
-        <v>0</v>
-      </c>
-      <c r="C36" s="4">
+      <c r="B36" s="5">
+        <v>0</v>
+      </c>
+      <c r="C36" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D36" s="5">
+      <c r="D36" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E36" s="6">
+      <c r="E36" s="5">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F36" s="4">
+      <c r="F36" s="3">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="G36" s="5">
+      <c r="G36" s="4">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -3264,27 +3268,27 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Q36" s="7">
+      <c r="Q36" s="6">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R36" s="9">
+      <c r="R36" s="8">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="S36" s="11">
+      <c r="S36" s="10">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="T36" s="7">
+      <c r="T36" s="6">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="U36" s="9">
+      <c r="U36" s="8">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="V36" s="11">
+      <c r="V36" s="10">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -3296,26 +3300,26 @@
       <c r="A37">
         <v>20</v>
       </c>
-      <c r="B37" s="6">
+      <c r="B37" s="5">
         <v>5</v>
       </c>
-      <c r="C37" s="4">
+      <c r="C37" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="D37" s="5">
+      <c r="D37" s="4">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="E37" s="6">
+      <c r="E37" s="5">
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-      <c r="F37" s="4">
+      <c r="F37" s="3">
         <f t="shared" si="12"/>
         <v>11</v>
       </c>
-      <c r="G37" s="5">
+      <c r="G37" s="4">
         <f t="shared" si="13"/>
         <v>16</v>
       </c>
@@ -3349,27 +3353,27 @@
         <f t="shared" si="4"/>
         <v>16.8</v>
       </c>
-      <c r="Q37" s="7">
+      <c r="Q37" s="6">
         <f t="shared" si="5"/>
         <v>5.25</v>
       </c>
-      <c r="R37" s="9">
+      <c r="R37" s="8">
         <f t="shared" si="6"/>
         <v>4.0999999999999996</v>
       </c>
-      <c r="S37" s="11">
+      <c r="S37" s="10">
         <f t="shared" si="7"/>
         <v>6.1499999999999995</v>
       </c>
-      <c r="T37" s="7">
+      <c r="T37" s="6">
         <f t="shared" si="8"/>
         <v>6.3000000000000007</v>
       </c>
-      <c r="U37" s="9">
+      <c r="U37" s="8">
         <f t="shared" si="9"/>
         <v>4.51</v>
       </c>
-      <c r="V37" s="11">
+      <c r="V37" s="10">
         <f t="shared" si="10"/>
         <v>6.56</v>
       </c>
@@ -3384,26 +3388,26 @@
       <c r="A38">
         <v>21</v>
       </c>
-      <c r="B38" s="6">
+      <c r="B38" s="5">
         <v>7</v>
       </c>
-      <c r="C38" s="4">
+      <c r="C38" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="D38" s="5">
+      <c r="D38" s="4">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="E38" s="6">
+      <c r="E38" s="5">
         <f t="shared" si="11"/>
         <v>8</v>
       </c>
-      <c r="F38" s="4">
+      <c r="F38" s="3">
         <f t="shared" si="12"/>
         <v>15</v>
       </c>
-      <c r="G38" s="5">
+      <c r="G38" s="4">
         <f t="shared" si="13"/>
         <v>22</v>
       </c>
@@ -3437,27 +3441,27 @@
         <f t="shared" si="4"/>
         <v>23.1</v>
       </c>
-      <c r="Q38" s="7">
+      <c r="Q38" s="6">
         <f t="shared" si="5"/>
         <v>7.3500000000000005</v>
       </c>
-      <c r="R38" s="9">
+      <c r="R38" s="8">
         <f t="shared" si="6"/>
         <v>5.7399999999999993</v>
       </c>
-      <c r="S38" s="11">
+      <c r="S38" s="10">
         <f t="shared" si="7"/>
         <v>8.61</v>
       </c>
-      <c r="T38" s="7">
+      <c r="T38" s="6">
         <f t="shared" si="8"/>
         <v>8.4</v>
       </c>
-      <c r="U38" s="9">
+      <c r="U38" s="8">
         <f t="shared" si="9"/>
         <v>6.1499999999999995</v>
       </c>
-      <c r="V38" s="11">
+      <c r="V38" s="10">
         <f t="shared" si="10"/>
         <v>9.02</v>
       </c>
@@ -3469,24 +3473,24 @@
       </c>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="B39" s="6"/>
-      <c r="C39" s="4">
+      <c r="B39" s="5"/>
+      <c r="C39" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D39" s="5">
+      <c r="D39" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E39" s="6">
+      <c r="E39" s="5">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F39" s="4">
+      <c r="F39" s="3">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="G39" s="5">
+      <c r="G39" s="4">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -3511,27 +3515,27 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Q39" s="7">
+      <c r="Q39" s="6">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R39" s="9">
+      <c r="R39" s="8">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="S39" s="11">
+      <c r="S39" s="10">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="T39" s="7">
+      <c r="T39" s="6">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="U39" s="9">
+      <c r="U39" s="8">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="V39" s="11">
+      <c r="V39" s="10">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -3540,26 +3544,26 @@
       <c r="A40">
         <v>22</v>
       </c>
-      <c r="B40" s="6">
-        <v>2</v>
-      </c>
-      <c r="C40" s="4">
+      <c r="B40" s="5">
+        <v>2</v>
+      </c>
+      <c r="C40" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D40" s="5">
+      <c r="D40" s="4">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="E40" s="6">
+      <c r="E40" s="5">
         <f t="shared" si="11"/>
         <v>3</v>
       </c>
-      <c r="F40" s="4">
+      <c r="F40" s="3">
         <f t="shared" si="12"/>
         <v>5</v>
       </c>
-      <c r="G40" s="5">
+      <c r="G40" s="4">
         <f t="shared" si="13"/>
         <v>7</v>
       </c>
@@ -3591,27 +3595,27 @@
         <f t="shared" si="4"/>
         <v>8.1199999999999992</v>
       </c>
-      <c r="Q40" s="7">
+      <c r="Q40" s="6">
         <f t="shared" si="5"/>
         <v>2.3199999999999998</v>
       </c>
-      <c r="R40" s="9">
+      <c r="R40" s="8">
         <f t="shared" si="6"/>
         <v>4.6399999999999997</v>
       </c>
-      <c r="S40" s="11">
+      <c r="S40" s="10">
         <f t="shared" si="7"/>
         <v>6.9599999999999991</v>
       </c>
-      <c r="T40" s="7">
+      <c r="T40" s="6">
         <f t="shared" si="8"/>
         <v>3.4799999999999995</v>
       </c>
-      <c r="U40" s="9">
+      <c r="U40" s="8">
         <f t="shared" si="9"/>
         <v>5.8</v>
       </c>
-      <c r="V40" s="11">
+      <c r="V40" s="10">
         <f t="shared" si="10"/>
         <v>8.1199999999999992</v>
       </c>
@@ -3626,26 +3630,26 @@
       <c r="A41">
         <v>23</v>
       </c>
-      <c r="B41" s="6">
-        <v>0</v>
-      </c>
-      <c r="C41" s="4">
+      <c r="B41" s="5">
+        <v>0</v>
+      </c>
+      <c r="C41" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D41" s="5">
+      <c r="D41" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E41" s="6">
+      <c r="E41" s="5">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F41" s="4">
+      <c r="F41" s="3">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="G41" s="5">
+      <c r="G41" s="4">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -3673,27 +3677,27 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Q41" s="7">
+      <c r="Q41" s="6">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R41" s="9">
+      <c r="R41" s="8">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="S41" s="11">
+      <c r="S41" s="10">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="T41" s="7">
+      <c r="T41" s="6">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="U41" s="9">
+      <c r="U41" s="8">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="V41" s="11">
+      <c r="V41" s="10">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -3702,26 +3706,26 @@
       <c r="A42">
         <v>24</v>
       </c>
-      <c r="B42" s="6">
-        <v>2</v>
-      </c>
-      <c r="C42" s="4">
+      <c r="B42" s="5">
+        <v>2</v>
+      </c>
+      <c r="C42" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D42" s="5">
+      <c r="D42" s="4">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="E42" s="6">
+      <c r="E42" s="5">
         <f t="shared" si="11"/>
         <v>3</v>
       </c>
-      <c r="F42" s="4">
+      <c r="F42" s="3">
         <f t="shared" si="12"/>
         <v>5</v>
       </c>
-      <c r="G42" s="5">
+      <c r="G42" s="4">
         <f t="shared" si="13"/>
         <v>7</v>
       </c>
@@ -3755,27 +3759,27 @@
         <f t="shared" si="4"/>
         <v>7.3500000000000005</v>
       </c>
-      <c r="Q42" s="7">
+      <c r="Q42" s="6">
         <f t="shared" si="5"/>
         <v>2.1</v>
       </c>
-      <c r="R42" s="9">
+      <c r="R42" s="8">
         <f t="shared" si="6"/>
         <v>4.2</v>
       </c>
-      <c r="S42" s="11">
+      <c r="S42" s="10">
         <f t="shared" si="7"/>
         <v>6.3000000000000007</v>
       </c>
-      <c r="T42" s="7">
+      <c r="T42" s="6">
         <f t="shared" si="8"/>
         <v>3.1500000000000004</v>
       </c>
-      <c r="U42" s="9">
+      <c r="U42" s="8">
         <f t="shared" si="9"/>
         <v>5.25</v>
       </c>
-      <c r="V42" s="11">
+      <c r="V42" s="10">
         <f t="shared" si="10"/>
         <v>7.3500000000000005</v>
       </c>
@@ -3790,26 +3794,26 @@
       <c r="A43">
         <v>25</v>
       </c>
-      <c r="B43" s="6">
+      <c r="B43" s="5">
         <v>1</v>
       </c>
-      <c r="C43" s="4">
+      <c r="C43" s="3">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D43" s="5">
+      <c r="D43" s="4">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="E43" s="6">
+      <c r="E43" s="5">
         <f t="shared" si="11"/>
         <v>2</v>
       </c>
-      <c r="F43" s="4">
+      <c r="F43" s="3">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="G43" s="5">
+      <c r="G43" s="4">
         <f t="shared" si="13"/>
         <v>4</v>
       </c>
@@ -3839,27 +3843,27 @@
         <f t="shared" si="4"/>
         <v>8.4</v>
       </c>
-      <c r="Q43" s="7">
+      <c r="Q43" s="6">
         <f t="shared" si="5"/>
         <v>2.1</v>
       </c>
-      <c r="R43" s="9">
+      <c r="R43" s="8">
         <f t="shared" si="6"/>
         <v>4.2</v>
       </c>
-      <c r="S43" s="11">
+      <c r="S43" s="10">
         <f t="shared" si="7"/>
         <v>6.3000000000000007</v>
       </c>
-      <c r="T43" s="7">
+      <c r="T43" s="6">
         <f t="shared" si="8"/>
         <v>4.2</v>
       </c>
-      <c r="U43" s="9">
+      <c r="U43" s="8">
         <f t="shared" si="9"/>
         <v>6.3000000000000007</v>
       </c>
-      <c r="V43" s="11">
+      <c r="V43" s="10">
         <f t="shared" si="10"/>
         <v>8.4</v>
       </c>
@@ -3874,26 +3878,26 @@
       <c r="A44">
         <v>26</v>
       </c>
-      <c r="B44" s="6">
-        <v>0</v>
-      </c>
-      <c r="C44" s="4">
+      <c r="B44" s="5">
+        <v>0</v>
+      </c>
+      <c r="C44" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D44" s="5">
+      <c r="D44" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E44" s="6">
+      <c r="E44" s="5">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F44" s="4">
+      <c r="F44" s="3">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="G44" s="5">
+      <c r="G44" s="4">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -3921,27 +3925,27 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Q44" s="7">
+      <c r="Q44" s="6">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R44" s="9">
+      <c r="R44" s="8">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="S44" s="11">
+      <c r="S44" s="10">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="T44" s="7">
+      <c r="T44" s="6">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="U44" s="9">
+      <c r="U44" s="8">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="V44" s="11">
+      <c r="V44" s="10">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -3953,26 +3957,26 @@
       <c r="A45">
         <v>27</v>
       </c>
-      <c r="B45" s="6">
+      <c r="B45" s="5">
         <v>1</v>
       </c>
-      <c r="C45" s="4">
+      <c r="C45" s="3">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D45" s="5">
+      <c r="D45" s="4">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="E45" s="6">
+      <c r="E45" s="5">
         <f t="shared" si="11"/>
         <v>2</v>
       </c>
-      <c r="F45" s="4">
+      <c r="F45" s="3">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="G45" s="5">
+      <c r="G45" s="4">
         <f t="shared" si="13"/>
         <v>4</v>
       </c>
@@ -4002,27 +4006,27 @@
         <f t="shared" si="4"/>
         <v>11.36</v>
       </c>
-      <c r="Q45" s="7">
+      <c r="Q45" s="6">
         <f t="shared" si="5"/>
         <v>2.84</v>
       </c>
-      <c r="R45" s="9">
+      <c r="R45" s="8">
         <f t="shared" si="6"/>
         <v>5.68</v>
       </c>
-      <c r="S45" s="11">
+      <c r="S45" s="10">
         <f t="shared" si="7"/>
         <v>8.52</v>
       </c>
-      <c r="T45" s="7">
+      <c r="T45" s="6">
         <f t="shared" si="8"/>
         <v>5.68</v>
       </c>
-      <c r="U45" s="9">
+      <c r="U45" s="8">
         <f t="shared" si="9"/>
         <v>8.52</v>
       </c>
-      <c r="V45" s="11">
+      <c r="V45" s="10">
         <f t="shared" si="10"/>
         <v>11.36</v>
       </c>
@@ -4037,26 +4041,26 @@
       <c r="A46">
         <v>28</v>
       </c>
-      <c r="B46" s="6">
+      <c r="B46" s="5">
         <v>1</v>
       </c>
-      <c r="C46" s="4">
+      <c r="C46" s="3">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D46" s="5">
+      <c r="D46" s="4">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="E46" s="6">
+      <c r="E46" s="5">
         <f t="shared" si="11"/>
         <v>2</v>
       </c>
-      <c r="F46" s="4">
+      <c r="F46" s="3">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="G46" s="5">
+      <c r="G46" s="4">
         <f t="shared" si="13"/>
         <v>4</v>
       </c>
@@ -4086,27 +4090,27 @@
         <f t="shared" si="4"/>
         <v>15.12</v>
       </c>
-      <c r="Q46" s="7">
+      <c r="Q46" s="6">
         <f t="shared" si="5"/>
         <v>3.78</v>
       </c>
-      <c r="R46" s="9">
+      <c r="R46" s="8">
         <f t="shared" si="6"/>
         <v>7.56</v>
       </c>
-      <c r="S46" s="11">
+      <c r="S46" s="10">
         <f t="shared" si="7"/>
         <v>11.34</v>
       </c>
-      <c r="T46" s="7">
+      <c r="T46" s="6">
         <f t="shared" si="8"/>
         <v>7.56</v>
       </c>
-      <c r="U46" s="9">
+      <c r="U46" s="8">
         <f t="shared" si="9"/>
         <v>11.34</v>
       </c>
-      <c r="V46" s="11">
+      <c r="V46" s="10">
         <f t="shared" si="10"/>
         <v>15.12</v>
       </c>
@@ -4121,26 +4125,26 @@
       <c r="A47">
         <v>29</v>
       </c>
-      <c r="B47" s="6">
-        <v>2</v>
-      </c>
-      <c r="C47" s="4">
+      <c r="B47" s="5">
+        <v>2</v>
+      </c>
+      <c r="C47" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D47" s="5">
+      <c r="D47" s="4">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="E47" s="6">
+      <c r="E47" s="5">
         <f t="shared" si="11"/>
         <v>3</v>
       </c>
-      <c r="F47" s="4">
+      <c r="F47" s="3">
         <f t="shared" si="12"/>
         <v>5</v>
       </c>
-      <c r="G47" s="5">
+      <c r="G47" s="4">
         <f t="shared" si="13"/>
         <v>7</v>
       </c>
@@ -4172,27 +4176,27 @@
         <f t="shared" si="4"/>
         <v>24.290000000000003</v>
       </c>
-      <c r="Q47" s="7">
+      <c r="Q47" s="6">
         <f t="shared" si="5"/>
         <v>6.94</v>
       </c>
-      <c r="R47" s="9">
+      <c r="R47" s="8">
         <f t="shared" si="6"/>
         <v>13.88</v>
       </c>
-      <c r="S47" s="11">
+      <c r="S47" s="10">
         <f t="shared" si="7"/>
         <v>20.82</v>
       </c>
-      <c r="T47" s="7">
+      <c r="T47" s="6">
         <f t="shared" si="8"/>
         <v>10.41</v>
       </c>
-      <c r="U47" s="9">
+      <c r="U47" s="8">
         <f t="shared" si="9"/>
         <v>17.350000000000001</v>
       </c>
-      <c r="V47" s="11">
+      <c r="V47" s="10">
         <f t="shared" si="10"/>
         <v>24.290000000000003</v>
       </c>
@@ -4207,28 +4211,25 @@
       <c r="A48">
         <v>30</v>
       </c>
-      <c r="B48" s="6">
+      <c r="B48" s="5">
         <v>1</v>
       </c>
-      <c r="C48" s="4">
+      <c r="C48" s="3">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D48" s="5">
+      <c r="D48" s="4">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="E48" s="6">
-        <f t="shared" si="11"/>
-        <v>2</v>
-      </c>
-      <c r="F48" s="4">
-        <f t="shared" si="12"/>
+      <c r="E48" s="5">
+        <v>1</v>
+      </c>
+      <c r="F48" s="3">
+        <v>2</v>
+      </c>
+      <c r="G48" s="4">
         <v>3</v>
-      </c>
-      <c r="G48" s="5">
-        <f t="shared" si="13"/>
-        <v>4</v>
       </c>
       <c r="I48" s="1" t="s">
         <v>130</v>
@@ -4252,31 +4253,31 @@
       </c>
       <c r="P48" s="2">
         <f t="shared" si="4"/>
-        <v>50.4</v>
-      </c>
-      <c r="Q48" s="7">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="Q48" s="6">
         <f t="shared" si="5"/>
         <v>12.6</v>
       </c>
-      <c r="R48" s="9">
+      <c r="R48" s="8">
         <f t="shared" si="6"/>
         <v>25.2</v>
       </c>
-      <c r="S48" s="11">
+      <c r="S48" s="10">
         <f t="shared" si="7"/>
         <v>37.799999999999997</v>
       </c>
-      <c r="T48" s="7">
+      <c r="T48" s="6">
         <f t="shared" si="8"/>
+        <v>12.6</v>
+      </c>
+      <c r="U48" s="8">
+        <f t="shared" si="9"/>
         <v>25.2</v>
       </c>
-      <c r="U48" s="9">
-        <f t="shared" si="9"/>
+      <c r="V48" s="10">
+        <f t="shared" si="10"/>
         <v>37.799999999999997</v>
-      </c>
-      <c r="V48" s="11">
-        <f t="shared" si="10"/>
-        <v>50.4</v>
       </c>
       <c r="W48" s="1" t="s">
         <v>130</v>
@@ -4286,32 +4287,32 @@
       </c>
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="B49" s="6">
+      <c r="B49" s="5">
         <f>SUM(B15:B48)</f>
         <v>71</v>
       </c>
-      <c r="C49" s="4">
+      <c r="C49" s="3">
         <f>SUM(C15:C48)</f>
         <v>142</v>
       </c>
-      <c r="D49" s="5">
+      <c r="D49" s="4">
         <f>SUM(D15:D48)</f>
         <v>213</v>
       </c>
-      <c r="E49" s="6">
+      <c r="E49" s="5">
         <f t="shared" ref="E49:G49" si="14">SUM(E15:E48)</f>
-        <v>88</v>
-      </c>
-      <c r="F49" s="4">
+        <v>86</v>
+      </c>
+      <c r="F49" s="3">
         <f t="shared" si="14"/>
-        <v>159</v>
-      </c>
-      <c r="G49" s="5">
+        <v>157</v>
+      </c>
+      <c r="G49" s="4">
         <f t="shared" si="14"/>
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
@@ -4329,88 +4330,88 @@
       </c>
       <c r="P49" s="2">
         <f t="shared" ref="P49:S49" si="15">SUM(P15:P48)</f>
-        <v>741.78</v>
-      </c>
-      <c r="Q49" s="7">
+        <v>729.18</v>
+      </c>
+      <c r="Q49" s="6">
         <f t="shared" si="15"/>
         <v>221.40299999999999</v>
       </c>
-      <c r="R49" s="9">
+      <c r="R49" s="8">
         <f t="shared" si="15"/>
         <v>427.44600000000003</v>
       </c>
-      <c r="S49" s="11">
+      <c r="S49" s="10">
         <f t="shared" si="15"/>
         <v>641.16899999999998</v>
       </c>
-      <c r="T49" s="7">
+      <c r="T49" s="6">
         <f t="shared" ref="T49:U49" si="16">SUM(T15:T48)</f>
-        <v>294.27700000000004</v>
-      </c>
-      <c r="U49" s="9">
+        <v>264.55700000000007</v>
+      </c>
+      <c r="U49" s="8">
         <f t="shared" si="16"/>
-        <v>499.04</v>
-      </c>
-      <c r="V49" s="11">
+        <v>469.32</v>
+      </c>
+      <c r="V49" s="10">
         <f>SUM(V15:V48)</f>
-        <v>690.70299999999997</v>
+        <v>678.10299999999995</v>
       </c>
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.35">
       <c r="J50" t="s">
         <v>116</v>
       </c>
-      <c r="Q50" s="7">
+      <c r="Q50" s="6">
         <f>Q49+IF(Q49&gt;=420,0,145)</f>
         <v>366.40300000000002</v>
       </c>
-      <c r="R50" s="9">
+      <c r="R50" s="8">
         <f t="shared" ref="R50:V50" si="17">R49+IF(R49&gt;=420,0,145)</f>
         <v>427.44600000000003</v>
       </c>
-      <c r="S50" s="11">
+      <c r="S50" s="10">
         <f t="shared" si="17"/>
         <v>641.16899999999998</v>
       </c>
-      <c r="T50" s="8">
+      <c r="T50" s="7">
         <f t="shared" ref="T50:U50" si="18">T49+IF(T49&gt;=420,0,145)</f>
-        <v>439.27700000000004</v>
-      </c>
-      <c r="U50" s="10">
+        <v>409.55700000000007</v>
+      </c>
+      <c r="U50" s="9">
         <f t="shared" si="18"/>
-        <v>499.04</v>
-      </c>
-      <c r="V50" s="12">
+        <v>469.32</v>
+      </c>
+      <c r="V50" s="11">
         <f t="shared" si="17"/>
-        <v>690.70299999999997</v>
+        <v>678.10299999999995</v>
       </c>
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
-      <c r="K51" s="3"/>
-      <c r="L51" s="3"/>
-      <c r="M51" s="3"/>
-      <c r="N51" s="3"/>
-      <c r="O51" s="3"/>
-      <c r="P51" s="3"/>
-      <c r="Q51" s="3"/>
-      <c r="R51" s="3"/>
-      <c r="S51" s="3"/>
-      <c r="T51" s="3"/>
-      <c r="U51" s="3"/>
-      <c r="V51" s="3"/>
-      <c r="W51" s="3"/>
-      <c r="X51" s="3"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="12"/>
+      <c r="H51" s="12"/>
+      <c r="I51" s="12"/>
+      <c r="J51" s="12"/>
+      <c r="K51" s="12"/>
+      <c r="L51" s="12"/>
+      <c r="M51" s="12"/>
+      <c r="N51" s="12"/>
+      <c r="O51" s="12"/>
+      <c r="P51" s="12"/>
+      <c r="Q51" s="12"/>
+      <c r="R51" s="12"/>
+      <c r="S51" s="12"/>
+      <c r="T51" s="12"/>
+      <c r="U51" s="12"/>
+      <c r="V51" s="12"/>
+      <c r="W51" s="12"/>
+      <c r="X51" s="12"/>
     </row>
     <row r="52" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A52">
@@ -4566,9 +4567,21 @@
   <mergeCells count="1">
     <mergeCell ref="B51:X51"/>
   </mergeCells>
-  <conditionalFormatting sqref="C49 A15:X48">
-    <cfRule type="expression" dxfId="0" priority="1">
+  <conditionalFormatting sqref="A15:X48 C49">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$B15=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J15:J48">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>